<commit_message>
merge 2023 and 2024 data
</commit_message>
<xml_diff>
--- a/raw-data/RSV Data 2024.xlsx
+++ b/raw-data/RSV Data 2024.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFEA9F46-8FDB-F645-BF4B-DF736037BE1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB30AF10-9909-6547-B68F-5E0498F5F290}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5420" yWindow="1060" windowWidth="24780" windowHeight="18620" activeTab="1" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
+    <workbookView xWindow="21220" yWindow="7280" windowWidth="24780" windowHeight="18620" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Papers" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$AC$71</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$O$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$O$53</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1407" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1566" uniqueCount="104">
   <si>
     <t>Trial</t>
   </si>
@@ -323,6 +324,36 @@
   </si>
   <si>
     <t>These are actually very severe</t>
+  </si>
+  <si>
+    <t>GSK</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arexvy </t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/ofid/article/9/Supplement_2/ofac492.312/6902559</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderna </t>
+  </si>
+  <si>
+    <t>Abs</t>
+  </si>
+  <si>
+    <t>MRNA-1345</t>
+  </si>
+  <si>
+    <t>2023 extraction</t>
+  </si>
+  <si>
+    <t>Bavarian Nordic</t>
+  </si>
+  <si>
+    <t>low</t>
+  </si>
+  <si>
+    <t>high</t>
   </si>
 </sst>
 </file>
@@ -1848,11 +1879,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8BCAD0-FE00-D14F-8109-AD4E81997C16}">
-  <dimension ref="A1:AC137"/>
+  <dimension ref="A1:AC149"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I133" sqref="I133"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7508,6 +7539,354 @@
         <v>10</v>
       </c>
     </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A138" t="s">
+        <v>86</v>
+      </c>
+      <c r="B138" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C138" t="s">
+        <v>39</v>
+      </c>
+      <c r="D138" t="s">
+        <v>86</v>
+      </c>
+      <c r="E138">
+        <v>0</v>
+      </c>
+      <c r="F138" t="s">
+        <v>8</v>
+      </c>
+      <c r="G138" t="s">
+        <v>16</v>
+      </c>
+      <c r="I138">
+        <v>1377.5604903874701</v>
+      </c>
+      <c r="K138" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A139" t="s">
+        <v>86</v>
+      </c>
+      <c r="B139" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C139" t="s">
+        <v>39</v>
+      </c>
+      <c r="D139" t="s">
+        <v>86</v>
+      </c>
+      <c r="E139">
+        <v>0</v>
+      </c>
+      <c r="F139" t="s">
+        <v>8</v>
+      </c>
+      <c r="G139" t="s">
+        <v>48</v>
+      </c>
+      <c r="I139">
+        <v>1153.9516206390899</v>
+      </c>
+      <c r="K139" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A140" t="s">
+        <v>86</v>
+      </c>
+      <c r="B140" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C140" t="s">
+        <v>39</v>
+      </c>
+      <c r="D140" t="s">
+        <v>86</v>
+      </c>
+      <c r="E140">
+        <v>30</v>
+      </c>
+      <c r="F140" t="s">
+        <v>8</v>
+      </c>
+      <c r="G140" t="s">
+        <v>48</v>
+      </c>
+      <c r="I140">
+        <v>13325.998891345</v>
+      </c>
+      <c r="K140" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A141" t="s">
+        <v>86</v>
+      </c>
+      <c r="B141" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C141" t="s">
+        <v>39</v>
+      </c>
+      <c r="D141" t="s">
+        <v>86</v>
+      </c>
+      <c r="E141">
+        <v>60</v>
+      </c>
+      <c r="F141" t="s">
+        <v>8</v>
+      </c>
+      <c r="G141" t="s">
+        <v>48</v>
+      </c>
+      <c r="I141">
+        <v>10419.607195087199</v>
+      </c>
+      <c r="K141" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A142" t="s">
+        <v>86</v>
+      </c>
+      <c r="B142" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C142" t="s">
+        <v>39</v>
+      </c>
+      <c r="D142" t="s">
+        <v>86</v>
+      </c>
+      <c r="E142">
+        <v>90</v>
+      </c>
+      <c r="F142" t="s">
+        <v>8</v>
+      </c>
+      <c r="G142" t="s">
+        <v>48</v>
+      </c>
+      <c r="I142">
+        <v>8746.5556943389493</v>
+      </c>
+      <c r="K142" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A143" t="s">
+        <v>86</v>
+      </c>
+      <c r="B143" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C143" t="s">
+        <v>39</v>
+      </c>
+      <c r="D143" t="s">
+        <v>86</v>
+      </c>
+      <c r="E143">
+        <v>180</v>
+      </c>
+      <c r="F143" t="s">
+        <v>8</v>
+      </c>
+      <c r="G143" t="s">
+        <v>48</v>
+      </c>
+      <c r="I143">
+        <v>5729.6814462350803</v>
+      </c>
+      <c r="K143" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A144" t="s">
+        <v>86</v>
+      </c>
+      <c r="B144" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C144" t="s">
+        <v>39</v>
+      </c>
+      <c r="D144" t="s">
+        <v>86</v>
+      </c>
+      <c r="E144">
+        <v>0</v>
+      </c>
+      <c r="F144" t="s">
+        <v>8</v>
+      </c>
+      <c r="G144" t="s">
+        <v>16</v>
+      </c>
+      <c r="I144">
+        <v>2113.6892331321401</v>
+      </c>
+      <c r="K144" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A145" t="s">
+        <v>86</v>
+      </c>
+      <c r="B145" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C145" t="s">
+        <v>39</v>
+      </c>
+      <c r="D145" t="s">
+        <v>86</v>
+      </c>
+      <c r="E145">
+        <v>0</v>
+      </c>
+      <c r="F145" t="s">
+        <v>8</v>
+      </c>
+      <c r="G145" t="s">
+        <v>48</v>
+      </c>
+      <c r="I145">
+        <v>1647.6610012426499</v>
+      </c>
+      <c r="K145" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A146" t="s">
+        <v>86</v>
+      </c>
+      <c r="B146" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C146" t="s">
+        <v>39</v>
+      </c>
+      <c r="D146" t="s">
+        <v>86</v>
+      </c>
+      <c r="E146">
+        <v>30</v>
+      </c>
+      <c r="F146" t="s">
+        <v>8</v>
+      </c>
+      <c r="G146" t="s">
+        <v>48</v>
+      </c>
+      <c r="I146">
+        <v>13947.175264341</v>
+      </c>
+      <c r="K146" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A147" t="s">
+        <v>86</v>
+      </c>
+      <c r="B147" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C147" t="s">
+        <v>39</v>
+      </c>
+      <c r="D147" t="s">
+        <v>86</v>
+      </c>
+      <c r="E147">
+        <v>60</v>
+      </c>
+      <c r="F147" t="s">
+        <v>8</v>
+      </c>
+      <c r="G147" t="s">
+        <v>48</v>
+      </c>
+      <c r="I147">
+        <v>11698.0459051707</v>
+      </c>
+      <c r="K147" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A148" t="s">
+        <v>86</v>
+      </c>
+      <c r="B148" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C148" t="s">
+        <v>39</v>
+      </c>
+      <c r="D148" t="s">
+        <v>86</v>
+      </c>
+      <c r="E148">
+        <v>90</v>
+      </c>
+      <c r="F148" t="s">
+        <v>8</v>
+      </c>
+      <c r="G148" t="s">
+        <v>48</v>
+      </c>
+      <c r="I148">
+        <v>9470.2519508610403</v>
+      </c>
+      <c r="K148" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A149" t="s">
+        <v>86</v>
+      </c>
+      <c r="B149" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C149" t="s">
+        <v>39</v>
+      </c>
+      <c r="D149" t="s">
+        <v>86</v>
+      </c>
+      <c r="E149">
+        <v>180</v>
+      </c>
+      <c r="F149" t="s">
+        <v>8</v>
+      </c>
+      <c r="G149" t="s">
+        <v>48</v>
+      </c>
+      <c r="I149">
+        <v>7944.2656978701298</v>
+      </c>
+      <c r="K149" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7516,11 +7895,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87136465-2DAE-EE48-9DCA-BA1E3F450528}">
-  <dimension ref="A1:N49"/>
+  <dimension ref="A1:N65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M28" sqref="M28"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58:J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8451,10 +8830,10 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B37" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C37" t="s">
         <v>52</v>
@@ -8463,36 +8842,24 @@
         <v>53</v>
       </c>
       <c r="G37">
-        <v>83.7</v>
+        <v>82.6</v>
       </c>
       <c r="H37">
-        <v>66</v>
+        <v>57.9</v>
       </c>
       <c r="I37">
-        <v>92.2</v>
+        <v>94.1</v>
       </c>
       <c r="J37" t="s">
         <v>55</v>
       </c>
-      <c r="K37">
-        <v>112</v>
-      </c>
-      <c r="L37" t="s">
-        <v>81</v>
-      </c>
-      <c r="M37" t="s">
-        <v>88</v>
-      </c>
-      <c r="N37" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B38" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C38" t="s">
         <v>52</v>
@@ -8501,142 +8868,78 @@
         <v>53</v>
       </c>
       <c r="G38">
-        <v>82.4</v>
+        <v>94.1</v>
       </c>
       <c r="H38">
-        <v>34.799999999999997</v>
+        <v>62.4</v>
       </c>
       <c r="I38">
-        <v>95.3</v>
+        <v>99.9</v>
       </c>
       <c r="J38" t="s">
-        <v>62</v>
-      </c>
-      <c r="K38">
-        <v>112</v>
-      </c>
-      <c r="L38" t="s">
-        <v>81</v>
-      </c>
-      <c r="M38" t="s">
-        <v>87</v>
-      </c>
-      <c r="N38" t="s">
-        <v>85</v>
+        <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B39" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C39" t="s">
         <v>52</v>
       </c>
       <c r="D39" t="s">
-        <v>53</v>
-      </c>
-      <c r="G39">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="H39">
-        <v>50.9</v>
-      </c>
-      <c r="I39">
-        <v>79.7</v>
-      </c>
-      <c r="J39" t="s">
-        <v>19</v>
-      </c>
-      <c r="K39">
-        <v>112</v>
-      </c>
-      <c r="L39" t="s">
-        <v>81</v>
-      </c>
-      <c r="M39" t="s">
-        <v>89</v>
-      </c>
-      <c r="N39" t="s">
-        <v>85</v>
+        <v>10</v>
+      </c>
+      <c r="E39">
+        <v>9329.7000000000007</v>
+      </c>
+      <c r="F39">
+        <v>928.6</v>
       </c>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B40" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C40" t="s">
         <v>52</v>
       </c>
       <c r="D40" t="s">
-        <v>10</v>
-      </c>
-      <c r="G40">
-        <v>91.7</v>
-      </c>
-      <c r="H40">
-        <v>73</v>
-      </c>
-      <c r="I40">
-        <v>97.4</v>
-      </c>
-      <c r="J40" t="s">
-        <v>55</v>
-      </c>
-      <c r="K40">
-        <v>112</v>
-      </c>
-      <c r="L40" t="s">
-        <v>81</v>
-      </c>
-      <c r="M40" t="s">
-        <v>88</v>
-      </c>
-      <c r="N40" t="s">
-        <v>85</v>
+        <v>11</v>
+      </c>
+      <c r="E40">
+        <v>10178.9</v>
+      </c>
+      <c r="F40">
+        <v>1124.0999999999999</v>
       </c>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="B41" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="C41" t="s">
         <v>52</v>
       </c>
       <c r="D41" t="s">
-        <v>10</v>
-      </c>
-      <c r="G41">
-        <v>90</v>
-      </c>
-      <c r="H41">
-        <v>22</v>
-      </c>
-      <c r="I41">
-        <v>98.7</v>
-      </c>
-      <c r="J41" t="s">
-        <v>62</v>
-      </c>
-      <c r="K41">
-        <v>112</v>
-      </c>
-      <c r="L41" t="s">
-        <v>81</v>
-      </c>
-      <c r="M41" t="s">
-        <v>87</v>
-      </c>
-      <c r="N41" t="s">
-        <v>85</v>
+        <v>53</v>
+      </c>
+      <c r="E41">
+        <f>GEOMEAN(E39:E40)</f>
+        <v>9745.0543010288038</v>
+      </c>
+      <c r="F41">
+        <f>GEOMEAN(F39:F40)</f>
+        <v>1021.6845207792862</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.2">
@@ -8650,16 +8953,16 @@
         <v>52</v>
       </c>
       <c r="D42" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="G42">
-        <v>68.5</v>
+        <v>83.7</v>
       </c>
       <c r="H42">
-        <v>21.1</v>
+        <v>66</v>
       </c>
       <c r="I42">
-        <v>87.4</v>
+        <v>92.2</v>
       </c>
       <c r="J42" t="s">
         <v>55</v>
@@ -8688,16 +8991,16 @@
         <v>52</v>
       </c>
       <c r="D43" t="s">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="G43">
-        <v>71.5</v>
+        <v>82.4</v>
       </c>
       <c r="H43">
-        <v>-37</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="I43">
-        <v>94.1</v>
+        <v>95.3</v>
       </c>
       <c r="J43" t="s">
         <v>62</v>
@@ -8720,25 +9023,37 @@
         <v>86</v>
       </c>
       <c r="B44" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C44" t="s">
         <v>52</v>
       </c>
       <c r="D44" t="s">
-        <v>10</v>
-      </c>
-      <c r="E44">
-        <v>8.3023429415730554</v>
-      </c>
-      <c r="F44">
-        <v>0.90097903892662778</v>
+        <v>53</v>
+      </c>
+      <c r="G44">
+        <v>68.400000000000006</v>
+      </c>
+      <c r="H44">
+        <v>50.9</v>
+      </c>
+      <c r="I44">
+        <v>79.7</v>
+      </c>
+      <c r="J44" t="s">
+        <v>19</v>
+      </c>
+      <c r="K44">
+        <v>112</v>
       </c>
       <c r="L44" t="s">
         <v>81</v>
       </c>
+      <c r="M44" t="s">
+        <v>89</v>
+      </c>
       <c r="N44" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.2">
@@ -8746,25 +9061,37 @@
         <v>86</v>
       </c>
       <c r="B45" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C45" t="s">
         <v>52</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
-      </c>
-      <c r="E45">
-        <v>11.392099607392703</v>
-      </c>
-      <c r="F45">
-        <v>1.1491516857651389</v>
+        <v>10</v>
+      </c>
+      <c r="G45">
+        <v>91.7</v>
+      </c>
+      <c r="H45">
+        <v>73</v>
+      </c>
+      <c r="I45">
+        <v>97.4</v>
+      </c>
+      <c r="J45" t="s">
+        <v>55</v>
+      </c>
+      <c r="K45">
+        <v>112</v>
       </c>
       <c r="L45" t="s">
         <v>81</v>
       </c>
+      <c r="M45" t="s">
+        <v>88</v>
+      </c>
       <c r="N45" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.2">
@@ -8772,27 +9099,37 @@
         <v>86</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C46" t="s">
         <v>52</v>
       </c>
       <c r="D46" t="s">
-        <v>53</v>
-      </c>
-      <c r="E46">
-        <f>GEOMEAN(E44:E45)</f>
-        <v>9.7252824002768161</v>
-      </c>
-      <c r="F46">
-        <f>GEOMEAN(F44:F45)</f>
-        <v>1.0175271895244811</v>
+        <v>10</v>
+      </c>
+      <c r="G46">
+        <v>90</v>
+      </c>
+      <c r="H46">
+        <v>22</v>
+      </c>
+      <c r="I46">
+        <v>98.7</v>
+      </c>
+      <c r="J46" t="s">
+        <v>62</v>
+      </c>
+      <c r="K46">
+        <v>112</v>
       </c>
       <c r="L46" t="s">
         <v>81</v>
       </c>
+      <c r="M46" t="s">
+        <v>87</v>
+      </c>
       <c r="N46" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.2">
@@ -8800,25 +9137,37 @@
         <v>86</v>
       </c>
       <c r="B47" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="D47" t="s">
-        <v>10</v>
-      </c>
-      <c r="E47">
-        <v>14.652591571562276</v>
-      </c>
-      <c r="F47">
-        <v>1.0888620819744395</v>
+        <v>11</v>
+      </c>
+      <c r="G47">
+        <v>68.5</v>
+      </c>
+      <c r="H47">
+        <v>21.1</v>
+      </c>
+      <c r="I47">
+        <v>87.4</v>
+      </c>
+      <c r="J47" t="s">
+        <v>55</v>
+      </c>
+      <c r="K47">
+        <v>112</v>
       </c>
       <c r="L47" t="s">
         <v>81</v>
       </c>
+      <c r="M47" t="s">
+        <v>88</v>
+      </c>
       <c r="N47" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.2">
@@ -8826,25 +9175,37 @@
         <v>86</v>
       </c>
       <c r="B48" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C48" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="D48" t="s">
         <v>11</v>
       </c>
-      <c r="E48">
-        <v>20.929300664290945</v>
-      </c>
-      <c r="F48">
-        <v>0.91677793244260819</v>
+      <c r="G48">
+        <v>71.5</v>
+      </c>
+      <c r="H48">
+        <v>-37</v>
+      </c>
+      <c r="I48">
+        <v>94.1</v>
+      </c>
+      <c r="J48" t="s">
+        <v>62</v>
+      </c>
+      <c r="K48">
+        <v>112</v>
       </c>
       <c r="L48" t="s">
         <v>81</v>
       </c>
+      <c r="M48" t="s">
+        <v>87</v>
+      </c>
       <c r="N48" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.2">
@@ -8855,28 +9216,424 @@
         <v>81</v>
       </c>
       <c r="C49" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
       <c r="D49" t="s">
-        <v>53</v>
+        <v>10</v>
       </c>
       <c r="E49">
-        <f>GEOMEAN(E47:E48)</f>
-        <v>17.511952904010514</v>
+        <v>8.3023429415730554</v>
       </c>
       <c r="F49">
-        <f>GEOMEAN(F47:F48)</f>
-        <v>0.99912197865309738</v>
+        <v>0.90097903892662778</v>
       </c>
       <c r="L49" t="s">
         <v>81</v>
       </c>
       <c r="N49" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>86</v>
+      </c>
+      <c r="B50" t="s">
+        <v>81</v>
+      </c>
+      <c r="C50" t="s">
+        <v>52</v>
+      </c>
+      <c r="D50" t="s">
+        <v>11</v>
+      </c>
+      <c r="E50">
+        <v>11.392099607392703</v>
+      </c>
+      <c r="F50">
+        <v>1.1491516857651389</v>
+      </c>
+      <c r="L50" t="s">
+        <v>81</v>
+      </c>
+      <c r="N50" t="s">
         <v>91</v>
       </c>
     </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" t="s">
+        <v>81</v>
+      </c>
+      <c r="C51" t="s">
+        <v>52</v>
+      </c>
+      <c r="D51" t="s">
+        <v>53</v>
+      </c>
+      <c r="E51">
+        <f>GEOMEAN(E49:E50)</f>
+        <v>9.7252824002768161</v>
+      </c>
+      <c r="F51">
+        <f>GEOMEAN(F49:F50)</f>
+        <v>1.0175271895244811</v>
+      </c>
+      <c r="L51" t="s">
+        <v>81</v>
+      </c>
+      <c r="N51" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" t="s">
+        <v>81</v>
+      </c>
+      <c r="C52" t="s">
+        <v>92</v>
+      </c>
+      <c r="D52" t="s">
+        <v>10</v>
+      </c>
+      <c r="E52">
+        <v>14.652591571562276</v>
+      </c>
+      <c r="F52">
+        <v>1.0888620819744395</v>
+      </c>
+      <c r="L52" t="s">
+        <v>81</v>
+      </c>
+      <c r="N52" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>86</v>
+      </c>
+      <c r="B53" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" t="s">
+        <v>92</v>
+      </c>
+      <c r="D53" t="s">
+        <v>11</v>
+      </c>
+      <c r="E53">
+        <v>20.929300664290945</v>
+      </c>
+      <c r="F53">
+        <v>0.91677793244260819</v>
+      </c>
+      <c r="L53" t="s">
+        <v>81</v>
+      </c>
+      <c r="N53" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>86</v>
+      </c>
+      <c r="B54" t="s">
+        <v>81</v>
+      </c>
+      <c r="C54" t="s">
+        <v>92</v>
+      </c>
+      <c r="D54" t="s">
+        <v>53</v>
+      </c>
+      <c r="E54">
+        <f>GEOMEAN(E52:E53)</f>
+        <v>17.511952904010514</v>
+      </c>
+      <c r="F54">
+        <f>GEOMEAN(F52:F53)</f>
+        <v>0.99912197865309738</v>
+      </c>
+      <c r="L54" t="s">
+        <v>81</v>
+      </c>
+      <c r="N54" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B55" t="s">
+        <v>99</v>
+      </c>
+      <c r="C55" t="s">
+        <v>52</v>
+      </c>
+      <c r="D55" t="s">
+        <v>10</v>
+      </c>
+      <c r="E55">
+        <v>13325.998891345</v>
+      </c>
+      <c r="F55">
+        <v>1377.5604903874701</v>
+      </c>
+      <c r="L55" t="s">
+        <v>81</v>
+      </c>
+      <c r="N55" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
+        <v>86</v>
+      </c>
+      <c r="B56" t="s">
+        <v>99</v>
+      </c>
+      <c r="C56" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
+      </c>
+      <c r="E56">
+        <v>13947.175264341</v>
+      </c>
+      <c r="F56">
+        <v>2113.6892331321401</v>
+      </c>
+      <c r="L56" t="s">
+        <v>81</v>
+      </c>
+      <c r="N56" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>86</v>
+      </c>
+      <c r="B57" t="s">
+        <v>99</v>
+      </c>
+      <c r="C57" t="s">
+        <v>52</v>
+      </c>
+      <c r="D57" t="s">
+        <v>53</v>
+      </c>
+      <c r="E57">
+        <f>GEOMEAN(E55:E56)</f>
+        <v>13633.049626184253</v>
+      </c>
+      <c r="F57">
+        <f>GEOMEAN(F55:F56)</f>
+        <v>1706.38060716835</v>
+      </c>
+      <c r="L57" t="s">
+        <v>81</v>
+      </c>
+      <c r="N57" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>101</v>
+      </c>
+      <c r="C58" t="s">
+        <v>52</v>
+      </c>
+      <c r="D58" t="s">
+        <v>53</v>
+      </c>
+      <c r="G58">
+        <v>59</v>
+      </c>
+      <c r="J58" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>101</v>
+      </c>
+      <c r="C59" t="s">
+        <v>52</v>
+      </c>
+      <c r="D59" t="s">
+        <v>53</v>
+      </c>
+      <c r="G59">
+        <v>42.9</v>
+      </c>
+      <c r="J59" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A60" t="s">
+        <v>101</v>
+      </c>
+      <c r="B60" t="s">
+        <v>102</v>
+      </c>
+      <c r="C60" t="s">
+        <v>52</v>
+      </c>
+      <c r="D60" t="s">
+        <v>10</v>
+      </c>
+      <c r="E60">
+        <v>316.7</v>
+      </c>
+      <c r="F60">
+        <v>251.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A61" t="s">
+        <v>101</v>
+      </c>
+      <c r="B61" t="s">
+        <v>102</v>
+      </c>
+      <c r="C61" t="s">
+        <v>52</v>
+      </c>
+      <c r="D61" t="s">
+        <v>11</v>
+      </c>
+      <c r="E61">
+        <v>517.70000000000005</v>
+      </c>
+      <c r="F61">
+        <v>477.5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A62" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" t="s">
+        <v>103</v>
+      </c>
+      <c r="C62" t="s">
+        <v>52</v>
+      </c>
+      <c r="D62" t="s">
+        <v>10</v>
+      </c>
+      <c r="E62">
+        <v>356.9</v>
+      </c>
+      <c r="F62">
+        <v>251.7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A63" t="s">
+        <v>101</v>
+      </c>
+      <c r="B63" t="s">
+        <v>103</v>
+      </c>
+      <c r="C63" t="s">
+        <v>52</v>
+      </c>
+      <c r="D63" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63">
+        <v>688.6</v>
+      </c>
+      <c r="F63">
+        <v>477.5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" t="s">
+        <v>102</v>
+      </c>
+      <c r="C64" t="s">
+        <v>52</v>
+      </c>
+      <c r="D64" t="s">
+        <v>53</v>
+      </c>
+      <c r="E64">
+        <f>GEOMEAN(E60:E61)</f>
+        <v>404.91429957461366</v>
+      </c>
+      <c r="F64">
+        <f>GEOMEAN(F60:F61)</f>
+        <v>346.67960713027236</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" t="s">
+        <v>103</v>
+      </c>
+      <c r="C65" t="s">
+        <v>52</v>
+      </c>
+      <c r="D65" t="s">
+        <v>53</v>
+      </c>
+      <c r="E65">
+        <f>GEOMEAN(E62:E63)</f>
+        <v>495.74321982252059</v>
+      </c>
+      <c r="F65">
+        <f>GEOMEAN(F62:F63)</f>
+        <v>346.67960713027236</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:O48" xr:uid="{87136465-2DAE-EE48-9DCA-BA1E3F450528}"/>
+  <autoFilter ref="A1:O53" xr:uid="{87136465-2DAE-EE48-9DCA-BA1E3F450528}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B96E09-4BF7-5E4A-9A2D-7FF2A0B754F5}">
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
include list of papers
</commit_message>
<xml_diff>
--- a/raw-data/RSV Data 2024.xlsx
+++ b/raw-data/RSV Data 2024.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z2211982/github/RSVcorrelates/raw-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC9BBBDF-3F2E-5547-8523-512FA9AC0F94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8388BA44-6D38-C14B-9E11-F25EE65B1422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6140" yWindow="1940" windowWidth="24780" windowHeight="18620" activeTab="3" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
   </bookViews>
@@ -597,24 +597,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -11396,7 +11386,7 @@
       <c r="H5" t="s">
         <v>112</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="I5" t="s">
         <v>110</v>
       </c>
     </row>
@@ -11596,97 +11586,97 @@
         <v>138</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="7" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="3" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+    <row r="3" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>142</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="6" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="4" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+    <row r="4" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>144</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="6" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="5" spans="1:3" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>147</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="7" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+    <row r="6" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="7" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="7" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>151</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="7" t="s">
         <v>150</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="6" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:3" s="8" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+    <row r="8" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>157</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="6" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="9" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="10" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="11" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="12" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="14" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="15" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
-    <row r="16" spans="1:3" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="12" t="s">
+    <row r="9" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="10" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="11" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="12" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="8" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="8" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
+    <row r="17" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="6" t="s">
         <v>155</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="6" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="8" t="s">
+    <row r="18" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="6" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="8" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>160</v>

</xml_diff>

<commit_message>
inlcude commentry on some novavax papers
</commit_message>
<xml_diff>
--- a/raw-data/RSV Data 2024.xlsx
+++ b/raw-data/RSV Data 2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8388BA44-6D38-C14B-9E11-F25EE65B1422}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5304844B-A5F4-C744-8E21-F2CEAC404C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="1940" windowWidth="24780" windowHeight="18620" activeTab="3" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
+    <workbookView xWindow="6140" yWindow="1940" windowWidth="24780" windowHeight="18620" activeTab="2" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="164">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1809" uniqueCount="173">
   <si>
     <t>Trial</t>
   </si>
@@ -441,9 +441,6 @@
     <t>data unsure</t>
   </si>
   <si>
-    <t>https://www.sciencedirect.com/science/article/pii/S0264410X17306813?via%3Dihub</t>
-  </si>
-  <si>
     <t>https://academic.oup.com/ofid/article/10/1/ofac693/6986211</t>
   </si>
   <si>
@@ -456,9 +453,6 @@
     <t>Novavax_preg_ab_JID2019</t>
   </si>
   <si>
-    <t>this shows very little effect of vaccine - is it a different vaccine?</t>
-  </si>
-  <si>
     <t>Mothers / Infants</t>
   </si>
   <si>
@@ -535,6 +529,39 @@
   </si>
   <si>
     <t>Prevention of Respiratory Syncytial Virus Infection: From Vaccine to Antibody</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/pii/S0264410X17306813</t>
+  </si>
+  <si>
+    <t>this shows very little effect of vaccine - and seems to be the same vaccine as Novavax_pref_abeff_NEJM2020</t>
+  </si>
+  <si>
+    <t>this shows strong immunological effect of vaccine and seems to be the same vaccine as Novavax_preg_ab_JID2019</t>
+  </si>
+  <si>
+    <t>RSV F nanoparticle vaccine</t>
+  </si>
+  <si>
+    <t>dose</t>
+  </si>
+  <si>
+    <t>120 μg of RSV F vaccine adsorbed to 0.4 mg of aluminum</t>
+  </si>
+  <si>
+    <t>Prepare</t>
+  </si>
+  <si>
+    <t>Analysis of data from Novavax_pref_abeff_NEJM2020</t>
+  </si>
+  <si>
+    <t>this is the first novavax study frm which they all follow</t>
+  </si>
+  <si>
+    <t>Figure 3</t>
+  </si>
+  <si>
+    <t>multiple</t>
   </si>
 </sst>
 </file>
@@ -597,7 +624,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -613,6 +640,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -7621,7 +7649,7 @@
     </row>
     <row r="102" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B102" t="s">
         <v>66</v>
@@ -7661,7 +7689,7 @@
     </row>
     <row r="103" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B103" t="s">
         <v>66</v>
@@ -7701,7 +7729,7 @@
     </row>
     <row r="104" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B104" t="s">
         <v>66</v>
@@ -7741,7 +7769,7 @@
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B105" t="s">
         <v>66</v>
@@ -7781,7 +7809,7 @@
     </row>
     <row r="106" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B106" t="s">
         <v>66</v>
@@ -7821,7 +7849,7 @@
     </row>
     <row r="107" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B107" t="s">
         <v>66</v>
@@ -7861,7 +7889,7 @@
     </row>
     <row r="108" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B108" t="s">
         <v>66</v>
@@ -7901,7 +7929,7 @@
     </row>
     <row r="109" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B109" t="s">
         <v>66</v>
@@ -7941,7 +7969,7 @@
     </row>
     <row r="110" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B110" t="s">
         <v>66</v>
@@ -7981,7 +8009,7 @@
     </row>
     <row r="111" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B111" t="s">
         <v>66</v>
@@ -8021,7 +8049,7 @@
     </row>
     <row r="112" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B112" t="s">
         <v>66</v>
@@ -8061,7 +8089,7 @@
     </row>
     <row r="113" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B113" t="s">
         <v>66</v>
@@ -8101,7 +8129,7 @@
     </row>
     <row r="114" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B114" t="s">
         <v>66</v>
@@ -8141,7 +8169,7 @@
     </row>
     <row r="115" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B115" t="s">
         <v>66</v>
@@ -8181,7 +8209,7 @@
     </row>
     <row r="116" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B116" t="s">
         <v>66</v>
@@ -8221,7 +8249,7 @@
     </row>
     <row r="117" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B117" t="s">
         <v>66</v>
@@ -8261,7 +8289,7 @@
     </row>
     <row r="118" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B118" t="s">
         <v>66</v>
@@ -8301,7 +8329,7 @@
     </row>
     <row r="119" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B119" t="s">
         <v>66</v>
@@ -8341,7 +8369,7 @@
     </row>
     <row r="120" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B120" t="s">
         <v>66</v>
@@ -8381,7 +8409,7 @@
     </row>
     <row r="121" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B121" t="s">
         <v>66</v>
@@ -8421,7 +8449,7 @@
     </row>
     <row r="122" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B122" t="s">
         <v>66</v>
@@ -8461,7 +8489,7 @@
     </row>
     <row r="123" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B123" t="s">
         <v>66</v>
@@ -8501,7 +8529,7 @@
     </row>
     <row r="124" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B124" t="s">
         <v>66</v>
@@ -8541,7 +8569,7 @@
     </row>
     <row r="125" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B125" t="s">
         <v>66</v>
@@ -8581,7 +8609,7 @@
     </row>
     <row r="126" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B126" t="s">
         <v>66</v>
@@ -11293,18 +11321,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B96E09-4BF7-5E4A-9A2D-7FF2A0B754F5}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>104</v>
       </c>
@@ -11315,25 +11344,28 @@
         <v>102</v>
       </c>
       <c r="D1" t="s">
+        <v>166</v>
+      </c>
+      <c r="E1" t="s">
         <v>47</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>100</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>62</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>105</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>71</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>103</v>
       </c>
@@ -11343,20 +11375,20 @@
       <c r="C2" t="s">
         <v>75</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>69</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>92</v>
       </c>
-      <c r="I2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="I3" s="4"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J3" s="4"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>107</v>
       </c>
@@ -11367,7 +11399,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>116</v>
       </c>
@@ -11377,20 +11409,20 @@
       <c r="C5" t="s">
         <v>108</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>111</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>92</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>112</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>117</v>
       </c>
@@ -11400,17 +11432,17 @@
       <c r="C6" t="s">
         <v>108</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>69</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>92</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>118</v>
       </c>
@@ -11420,20 +11452,20 @@
       <c r="C7" t="s">
         <v>108</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>67</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>119</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>127</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>122</v>
       </c>
@@ -11443,125 +11475,173 @@
       <c r="C8" t="s">
         <v>108</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>69</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>119</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>128</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>66</v>
       </c>
       <c r="B9" t="s">
         <v>66</v>
       </c>
+      <c r="C9" t="s">
+        <v>165</v>
+      </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>172</v>
       </c>
       <c r="E9" t="s">
+        <v>109</v>
+      </c>
+      <c r="F9" t="s">
         <v>125</v>
       </c>
-      <c r="G9" t="s">
-        <v>124</v>
+      <c r="H9" t="s">
+        <v>171</v>
       </c>
       <c r="I9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>135</v>
       </c>
       <c r="B10" t="s">
         <v>66</v>
       </c>
+      <c r="C10" t="s">
+        <v>165</v>
+      </c>
       <c r="D10" t="s">
-        <v>69</v>
+        <v>167</v>
       </c>
       <c r="E10" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="F10" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="I10" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>66</v>
+        <v>126</v>
       </c>
       <c r="B11" t="s">
         <v>66</v>
       </c>
+      <c r="C11" t="s">
+        <v>165</v>
+      </c>
       <c r="D11" t="s">
-        <v>109</v>
+        <v>167</v>
       </c>
       <c r="E11" t="s">
+        <v>111</v>
+      </c>
+      <c r="F11" t="s">
         <v>125</v>
       </c>
+      <c r="G11" t="s">
+        <v>168</v>
+      </c>
+      <c r="H11" t="s">
+        <v>124</v>
+      </c>
       <c r="I11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>66</v>
       </c>
+      <c r="C12" t="s">
+        <v>165</v>
+      </c>
       <c r="D12" t="s">
+        <v>167</v>
+      </c>
+      <c r="E12" t="s">
         <v>111</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>125</v>
       </c>
+      <c r="G12" t="s">
+        <v>168</v>
+      </c>
       <c r="I12" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>66</v>
+      </c>
       <c r="B13" t="s">
         <v>66</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>69</v>
       </c>
-      <c r="E13" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>136</v>
-      </c>
+      <c r="F13" t="s">
+        <v>119</v>
+      </c>
+      <c r="G13" t="s">
+        <v>130</v>
+      </c>
+      <c r="J13" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>66</v>
       </c>
-      <c r="D14" t="s">
-        <v>111</v>
-      </c>
       <c r="E14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
         <v>92</v>
       </c>
-      <c r="H14" t="s">
-        <v>137</v>
-      </c>
-      <c r="I14" t="s">
-        <v>135</v>
+      <c r="J14" t="s">
+        <v>133</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J11" r:id="rId1" xr:uid="{FBBA50AB-2952-9F43-883D-9A11D2D39C86}"/>
+    <hyperlink ref="J9" r:id="rId2" xr:uid="{F0CF3696-1BA1-5C43-9863-A926EBA2EA13}"/>
+    <hyperlink ref="J10" r:id="rId3" xr:uid="{EAD1F518-105F-A543-A35F-D9623B74AF78}"/>
+    <hyperlink ref="J12" r:id="rId4" xr:uid="{6E80B355-568F-5044-97B9-11158FDCBA4C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -11570,8 +11650,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC9BE8B-F6ED-034E-98E8-60BCAE861F6C}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11583,69 +11663,69 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A4" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C4" s="6" t="s">
         <v>143</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="C7" s="6" t="s">
         <v>150</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="6" customFormat="1" ht="34" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
@@ -11657,40 +11737,40 @@
     <row r="15" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="16" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="8" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="17" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B17" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>154</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B18" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2"/>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B22" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C22" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
include more up to date data
</commit_message>
<xml_diff>
--- a/raw-data/RSV Data 2024.xlsx
+++ b/raw-data/RSV Data 2024.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5A15AB-2A3E-764D-9C50-280DE15AA9F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9896ABCC-5D01-0549-AA1A-789A3E0D27E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="1940" windowWidth="24780" windowHeight="18620" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
+    <workbookView xWindow="6140" yWindow="1940" windowWidth="24780" windowHeight="18620" activeTab="2" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibodies" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ab_eff" sheetId="2" r:id="rId2"/>
     <sheet name="Papers" sheetId="3" r:id="rId3"/>
     <sheet name="Natural Abs" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">ab_eff!$B$1:$P$65</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Antibodies!$A$1:$AH$177</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$B$1:$P$65</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2082" uniqueCount="181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="205">
   <si>
     <t>Trial</t>
   </si>
@@ -586,6 +586,78 @@
   </si>
   <si>
     <t>delivery</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41591-023-02316-5</t>
+  </si>
+  <si>
+    <t>MELODY, Phase2b</t>
+  </si>
+  <si>
+    <t>AzSanofi_infants_abeff_combined_NatMed2023</t>
+  </si>
+  <si>
+    <t>AzSanofi_infants_eff_MELODY_NEJM2022</t>
+  </si>
+  <si>
+    <t>https://www.nejm.org/doi/10.1056/NEJMoa2110275</t>
+  </si>
+  <si>
+    <t>AzSanofi_infants_eff_Phase2b_NEJM2020</t>
+  </si>
+  <si>
+    <t>https://www.nejm.org/doi/full/10.1056/nejmoa1913556</t>
+  </si>
+  <si>
+    <t>BavarianNordic_elderly_eff_News2023</t>
+  </si>
+  <si>
+    <t>https://www.bavarian-nordic.com/investor/news/news.aspx?news=6808</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jid/article/228/8/999/7133623</t>
+  </si>
+  <si>
+    <t>abs</t>
+  </si>
+  <si>
+    <t>BavarianNordic</t>
+  </si>
+  <si>
+    <t>adults</t>
+  </si>
+  <si>
+    <t>HumanChallenge</t>
+  </si>
+  <si>
+    <t>BavarianNordic_adults_abchallenge_JID2023</t>
+  </si>
+  <si>
+    <t>https://academic.oup.com/jid/article/223/6/1062/5878073</t>
+  </si>
+  <si>
+    <t>MVA-BN-RSV</t>
+  </si>
+  <si>
+    <t>1 × 10^8 InfU</t>
+  </si>
+  <si>
+    <t>5 × 10^8 InfU</t>
+  </si>
+  <si>
+    <t>BavarianNordic_adults_ab_JID2021</t>
+  </si>
+  <si>
+    <t>low dose (only)</t>
+  </si>
+  <si>
+    <t>low dose (+later dose)</t>
+  </si>
+  <si>
+    <t>high dose (only)</t>
+  </si>
+  <si>
+    <t>high dose (+later dose)</t>
   </si>
 </sst>
 </file>
@@ -595,7 +667,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -622,6 +694,18 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -654,7 +738,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -670,9 +754,19 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2148,15 +2242,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF8BCAD0-FE00-D14F-8109-AD4E81997C16}">
-  <dimension ref="A1:AH177"/>
+  <dimension ref="A1:AH241"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A139" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K156" sqref="K156:K161"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A192" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K229" sqref="K229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="30" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="13.83203125" customWidth="1"/>
     <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -6951,7 +7046,7 @@
         <v>58</v>
       </c>
       <c r="H77">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="I77" t="s">
         <v>9</v>
@@ -7247,7 +7342,7 @@
         <v>58</v>
       </c>
       <c r="H85">
-        <v>91</v>
+        <v>31</v>
       </c>
       <c r="I85" t="s">
         <v>9</v>
@@ -9777,15 +9872,15 @@
         <v>Novavax</v>
       </c>
       <c r="D150" t="s">
+        <v>109</v>
+      </c>
+      <c r="E150" t="s">
         <v>177</v>
       </c>
-      <c r="E150" t="s">
-        <v>68</v>
-      </c>
       <c r="F150" t="s">
         <v>36</v>
       </c>
-      <c r="G150" s="11" t="s">
+      <c r="G150" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H150">
@@ -9797,7 +9892,7 @@
       <c r="J150" t="s">
         <v>45</v>
       </c>
-      <c r="K150" s="11" t="s">
+      <c r="K150" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L150">
@@ -9825,15 +9920,15 @@
         <v>Novavax</v>
       </c>
       <c r="D151" t="s">
+        <v>109</v>
+      </c>
+      <c r="E151" t="s">
         <v>177</v>
       </c>
-      <c r="E151" t="s">
-        <v>68</v>
-      </c>
       <c r="F151" t="s">
         <v>36</v>
       </c>
-      <c r="G151" s="11" t="s">
+      <c r="G151" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H151">
@@ -9845,7 +9940,7 @@
       <c r="J151" t="s">
         <v>45</v>
       </c>
-      <c r="K151" s="11" t="s">
+      <c r="K151" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L151">
@@ -9873,15 +9968,15 @@
         <v>Novavax</v>
       </c>
       <c r="D152" t="s">
+        <v>109</v>
+      </c>
+      <c r="E152" t="s">
         <v>177</v>
       </c>
-      <c r="E152" t="s">
-        <v>68</v>
-      </c>
       <c r="F152" t="s">
         <v>36</v>
       </c>
-      <c r="G152" s="11" t="s">
+      <c r="G152" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H152">
@@ -9893,7 +9988,7 @@
       <c r="J152" t="s">
         <v>45</v>
       </c>
-      <c r="K152" s="11" t="s">
+      <c r="K152" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L152">
@@ -9921,15 +10016,15 @@
         <v>Novavax</v>
       </c>
       <c r="D153" t="s">
+        <v>109</v>
+      </c>
+      <c r="E153" t="s">
         <v>177</v>
       </c>
-      <c r="E153" t="s">
-        <v>68</v>
-      </c>
       <c r="F153" t="s">
         <v>36</v>
       </c>
-      <c r="G153" s="11" t="s">
+      <c r="G153" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H153">
@@ -9941,7 +10036,7 @@
       <c r="J153" t="s">
         <v>45</v>
       </c>
-      <c r="K153" s="11" t="s">
+      <c r="K153" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L153">
@@ -9969,15 +10064,15 @@
         <v>Novavax</v>
       </c>
       <c r="D154" t="s">
+        <v>109</v>
+      </c>
+      <c r="E154" t="s">
         <v>177</v>
       </c>
-      <c r="E154" t="s">
-        <v>68</v>
-      </c>
       <c r="F154" t="s">
         <v>36</v>
       </c>
-      <c r="G154" s="11" t="s">
+      <c r="G154" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H154">
@@ -9989,7 +10084,7 @@
       <c r="J154" t="s">
         <v>45</v>
       </c>
-      <c r="K154" s="11" t="s">
+      <c r="K154" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L154">
@@ -10017,15 +10112,15 @@
         <v>Novavax</v>
       </c>
       <c r="D155" t="s">
+        <v>109</v>
+      </c>
+      <c r="E155" t="s">
         <v>177</v>
       </c>
-      <c r="E155" t="s">
-        <v>68</v>
-      </c>
       <c r="F155" t="s">
         <v>36</v>
       </c>
-      <c r="G155" s="11" t="s">
+      <c r="G155" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H155">
@@ -10037,7 +10132,7 @@
       <c r="J155" t="s">
         <v>45</v>
       </c>
-      <c r="K155" s="11" t="s">
+      <c r="K155" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L155">
@@ -10065,15 +10160,15 @@
         <v>Novavax</v>
       </c>
       <c r="D156" t="s">
+        <v>109</v>
+      </c>
+      <c r="E156" t="s">
         <v>177</v>
       </c>
-      <c r="E156" t="s">
-        <v>68</v>
-      </c>
       <c r="F156" t="s">
         <v>36</v>
       </c>
-      <c r="G156" s="11" t="s">
+      <c r="G156" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H156">
@@ -10085,7 +10180,7 @@
       <c r="J156" t="s">
         <v>16</v>
       </c>
-      <c r="K156" s="11"/>
+      <c r="K156" s="12"/>
       <c r="L156">
         <v>225.82758147402399</v>
       </c>
@@ -10111,15 +10206,15 @@
         <v>Novavax</v>
       </c>
       <c r="D157" t="s">
+        <v>109</v>
+      </c>
+      <c r="E157" t="s">
         <v>177</v>
       </c>
-      <c r="E157" t="s">
-        <v>68</v>
-      </c>
       <c r="F157" t="s">
         <v>36</v>
       </c>
-      <c r="G157" s="11" t="s">
+      <c r="G157" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H157">
@@ -10131,7 +10226,7 @@
       <c r="J157" t="s">
         <v>16</v>
       </c>
-      <c r="K157" s="11"/>
+      <c r="K157" s="12"/>
       <c r="L157">
         <v>236.93586718735</v>
       </c>
@@ -10157,15 +10252,15 @@
         <v>Novavax</v>
       </c>
       <c r="D158" t="s">
+        <v>109</v>
+      </c>
+      <c r="E158" t="s">
         <v>177</v>
       </c>
-      <c r="E158" t="s">
-        <v>68</v>
-      </c>
       <c r="F158" t="s">
         <v>36</v>
       </c>
-      <c r="G158" s="11" t="s">
+      <c r="G158" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H158">
@@ -10177,7 +10272,7 @@
       <c r="J158" t="s">
         <v>16</v>
       </c>
-      <c r="K158" s="11"/>
+      <c r="K158" s="12"/>
       <c r="L158">
         <v>241.48529086561999</v>
       </c>
@@ -10203,15 +10298,15 @@
         <v>Novavax</v>
       </c>
       <c r="D159" t="s">
+        <v>109</v>
+      </c>
+      <c r="E159" t="s">
         <v>177</v>
       </c>
-      <c r="E159" t="s">
-        <v>68</v>
-      </c>
       <c r="F159" t="s">
         <v>36</v>
       </c>
-      <c r="G159" s="11" t="s">
+      <c r="G159" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H159">
@@ -10223,7 +10318,7 @@
       <c r="J159" t="s">
         <v>16</v>
       </c>
-      <c r="K159" s="11"/>
+      <c r="K159" s="12"/>
       <c r="L159">
         <v>313.95626619498898</v>
       </c>
@@ -10249,15 +10344,15 @@
         <v>Novavax</v>
       </c>
       <c r="D160" t="s">
+        <v>109</v>
+      </c>
+      <c r="E160" t="s">
         <v>177</v>
       </c>
-      <c r="E160" t="s">
-        <v>68</v>
-      </c>
       <c r="F160" t="s">
         <v>36</v>
       </c>
-      <c r="G160" s="11" t="s">
+      <c r="G160" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H160">
@@ -10269,7 +10364,7 @@
       <c r="J160" t="s">
         <v>16</v>
       </c>
-      <c r="K160" s="11"/>
+      <c r="K160" s="12"/>
       <c r="L160">
         <v>291.26267903046897</v>
       </c>
@@ -10295,15 +10390,15 @@
         <v>Novavax</v>
       </c>
       <c r="D161" t="s">
+        <v>109</v>
+      </c>
+      <c r="E161" t="s">
         <v>177</v>
       </c>
-      <c r="E161" t="s">
-        <v>68</v>
-      </c>
       <c r="F161" t="s">
         <v>36</v>
       </c>
-      <c r="G161" s="11" t="s">
+      <c r="G161" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H161">
@@ -10315,7 +10410,7 @@
       <c r="J161" t="s">
         <v>16</v>
       </c>
-      <c r="K161" s="11"/>
+      <c r="K161" s="12"/>
       <c r="L161">
         <v>290.82615161212198</v>
       </c>
@@ -10349,7 +10444,7 @@
       <c r="F162" t="s">
         <v>36</v>
       </c>
-      <c r="G162" s="11" t="s">
+      <c r="G162" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H162">
@@ -10361,7 +10456,7 @@
       <c r="J162" t="s">
         <v>16</v>
       </c>
-      <c r="K162" s="11"/>
+      <c r="K162" s="12"/>
       <c r="L162">
         <v>665</v>
       </c>
@@ -10386,7 +10481,7 @@
         <v>66</v>
       </c>
       <c r="C163" t="str">
-        <f t="shared" ref="C163:C177" si="21">B163</f>
+        <f t="shared" ref="C163:C178" si="21">B163</f>
         <v>Novavax</v>
       </c>
       <c r="D163" t="s">
@@ -10398,7 +10493,7 @@
       <c r="F163" t="s">
         <v>36</v>
       </c>
-      <c r="G163" s="11" t="s">
+      <c r="G163" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H163">
@@ -10410,7 +10505,7 @@
       <c r="J163" t="s">
         <v>45</v>
       </c>
-      <c r="K163" s="11" t="s">
+      <c r="K163" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L163">
@@ -10449,7 +10544,7 @@
       <c r="F164" t="s">
         <v>36</v>
       </c>
-      <c r="G164" s="11" t="s">
+      <c r="G164" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H164">
@@ -10461,7 +10556,7 @@
       <c r="J164" t="s">
         <v>16</v>
       </c>
-      <c r="K164" s="11"/>
+      <c r="K164" s="12"/>
       <c r="L164">
         <v>883</v>
       </c>
@@ -10498,7 +10593,7 @@
       <c r="F165" t="s">
         <v>36</v>
       </c>
-      <c r="G165" s="11" t="s">
+      <c r="G165" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H165">
@@ -10510,7 +10605,7 @@
       <c r="J165" t="s">
         <v>45</v>
       </c>
-      <c r="K165" s="11" t="s">
+      <c r="K165" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L165">
@@ -10549,7 +10644,7 @@
       <c r="F166" t="s">
         <v>36</v>
       </c>
-      <c r="G166" s="11" t="s">
+      <c r="G166" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H166">
@@ -10561,7 +10656,7 @@
       <c r="J166" t="s">
         <v>16</v>
       </c>
-      <c r="K166" s="11"/>
+      <c r="K166" s="12"/>
       <c r="L166">
         <v>654</v>
       </c>
@@ -10598,7 +10693,7 @@
       <c r="F167" t="s">
         <v>36</v>
       </c>
-      <c r="G167" s="11" t="s">
+      <c r="G167" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H167">
@@ -10610,7 +10705,7 @@
       <c r="J167" t="s">
         <v>45</v>
       </c>
-      <c r="K167" s="11" t="s">
+      <c r="K167" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L167">
@@ -10649,7 +10744,7 @@
       <c r="F168" t="s">
         <v>36</v>
       </c>
-      <c r="G168" s="11" t="s">
+      <c r="G168" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H168">
@@ -10661,7 +10756,7 @@
       <c r="J168" t="s">
         <v>16</v>
       </c>
-      <c r="K168" s="11"/>
+      <c r="K168" s="12"/>
       <c r="L168">
         <v>845</v>
       </c>
@@ -10698,7 +10793,7 @@
       <c r="F169" t="s">
         <v>36</v>
       </c>
-      <c r="G169" s="11" t="s">
+      <c r="G169" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H169">
@@ -10710,7 +10805,7 @@
       <c r="J169" t="s">
         <v>45</v>
       </c>
-      <c r="K169" s="11" t="s">
+      <c r="K169" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L169">
@@ -10749,7 +10844,7 @@
       <c r="F170" t="s">
         <v>36</v>
       </c>
-      <c r="G170" s="11" t="s">
+      <c r="G170" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H170">
@@ -10761,7 +10856,7 @@
       <c r="J170" t="s">
         <v>16</v>
       </c>
-      <c r="K170" s="11"/>
+      <c r="K170" s="12"/>
       <c r="L170">
         <v>589</v>
       </c>
@@ -10798,7 +10893,7 @@
       <c r="F171" t="s">
         <v>36</v>
       </c>
-      <c r="G171" s="11" t="s">
+      <c r="G171" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H171">
@@ -10810,7 +10905,7 @@
       <c r="J171" t="s">
         <v>45</v>
       </c>
-      <c r="K171" s="11" t="s">
+      <c r="K171" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L171">
@@ -10849,7 +10944,7 @@
       <c r="F172" t="s">
         <v>36</v>
       </c>
-      <c r="G172" s="11" t="s">
+      <c r="G172" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H172">
@@ -10861,7 +10956,7 @@
       <c r="J172" t="s">
         <v>16</v>
       </c>
-      <c r="K172" s="11"/>
+      <c r="K172" s="12"/>
       <c r="L172">
         <v>592</v>
       </c>
@@ -10898,7 +10993,7 @@
       <c r="F173" t="s">
         <v>36</v>
       </c>
-      <c r="G173" s="11" t="s">
+      <c r="G173" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H173">
@@ -10910,7 +11005,7 @@
       <c r="J173" t="s">
         <v>45</v>
       </c>
-      <c r="K173" s="11" t="s">
+      <c r="K173" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L173">
@@ -10949,7 +11044,7 @@
       <c r="F174" t="s">
         <v>36</v>
       </c>
-      <c r="G174" s="11" t="s">
+      <c r="G174" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H174">
@@ -10961,7 +11056,7 @@
       <c r="J174" t="s">
         <v>16</v>
       </c>
-      <c r="K174" s="11"/>
+      <c r="K174" s="12"/>
       <c r="L174">
         <v>732</v>
       </c>
@@ -10998,7 +11093,7 @@
       <c r="F175" t="s">
         <v>36</v>
       </c>
-      <c r="G175" s="11" t="s">
+      <c r="G175" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H175">
@@ -11010,7 +11105,7 @@
       <c r="J175" t="s">
         <v>45</v>
       </c>
-      <c r="K175" s="11" t="s">
+      <c r="K175" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L175">
@@ -11049,7 +11144,7 @@
       <c r="F176" t="s">
         <v>36</v>
       </c>
-      <c r="G176" s="11" t="s">
+      <c r="G176" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H176">
@@ -11061,7 +11156,7 @@
       <c r="J176" t="s">
         <v>16</v>
       </c>
-      <c r="K176" s="11"/>
+      <c r="K176" s="12"/>
       <c r="L176">
         <v>607</v>
       </c>
@@ -11098,7 +11193,7 @@
       <c r="F177" t="s">
         <v>36</v>
       </c>
-      <c r="G177" s="11" t="s">
+      <c r="G177" s="12" t="s">
         <v>179</v>
       </c>
       <c r="H177">
@@ -11110,7 +11205,7 @@
       <c r="J177" t="s">
         <v>45</v>
       </c>
-      <c r="K177" s="11" t="s">
+      <c r="K177" s="12" t="s">
         <v>165</v>
       </c>
       <c r="L177">
@@ -11129,8 +11224,3241 @@
         <v>757</v>
       </c>
     </row>
+    <row r="178" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A178" t="s">
+        <v>200</v>
+      </c>
+      <c r="B178" t="s">
+        <v>192</v>
+      </c>
+      <c r="C178" t="str">
+        <f t="shared" si="21"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D178" t="s">
+        <v>69</v>
+      </c>
+      <c r="E178" t="s">
+        <v>201</v>
+      </c>
+      <c r="F178" t="s">
+        <v>36</v>
+      </c>
+      <c r="G178" t="s">
+        <v>197</v>
+      </c>
+      <c r="H178">
+        <v>0</v>
+      </c>
+      <c r="I178" t="s">
+        <v>8</v>
+      </c>
+      <c r="J178" t="s">
+        <v>45</v>
+      </c>
+      <c r="K178" t="s">
+        <v>198</v>
+      </c>
+      <c r="L178" s="14">
+        <v>256.39999999999998</v>
+      </c>
+      <c r="M178" s="15"/>
+      <c r="N178" s="14">
+        <v>214.2</v>
+      </c>
+      <c r="O178">
+        <v>307</v>
+      </c>
+      <c r="P178" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q178" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="179" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A179" t="s">
+        <v>200</v>
+      </c>
+      <c r="B179" t="s">
+        <v>192</v>
+      </c>
+      <c r="C179" t="str">
+        <f t="shared" ref="C179:C217" si="22">B179</f>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D179" t="s">
+        <v>69</v>
+      </c>
+      <c r="E179" t="s">
+        <v>201</v>
+      </c>
+      <c r="F179" t="s">
+        <v>36</v>
+      </c>
+      <c r="G179" t="s">
+        <v>197</v>
+      </c>
+      <c r="H179">
+        <v>0</v>
+      </c>
+      <c r="I179" t="s">
+        <v>8</v>
+      </c>
+      <c r="J179" t="s">
+        <v>45</v>
+      </c>
+      <c r="K179" t="s">
+        <v>198</v>
+      </c>
+      <c r="L179" s="14">
+        <v>424.3</v>
+      </c>
+      <c r="M179" s="15"/>
+      <c r="N179" s="14">
+        <v>332</v>
+      </c>
+      <c r="O179">
+        <v>542.20000000000005</v>
+      </c>
+      <c r="P179" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q179" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="180" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A180" t="s">
+        <v>200</v>
+      </c>
+      <c r="B180" t="s">
+        <v>192</v>
+      </c>
+      <c r="C180" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D180" t="s">
+        <v>69</v>
+      </c>
+      <c r="E180" t="s">
+        <v>201</v>
+      </c>
+      <c r="F180" t="s">
+        <v>36</v>
+      </c>
+      <c r="G180" t="s">
+        <v>197</v>
+      </c>
+      <c r="H180">
+        <v>14</v>
+      </c>
+      <c r="I180" t="s">
+        <v>8</v>
+      </c>
+      <c r="J180" t="s">
+        <v>45</v>
+      </c>
+      <c r="K180" t="s">
+        <v>198</v>
+      </c>
+      <c r="L180" s="14">
+        <v>316.7</v>
+      </c>
+      <c r="M180" s="15"/>
+      <c r="N180" s="14">
+        <v>266.3</v>
+      </c>
+      <c r="O180">
+        <v>376.6</v>
+      </c>
+      <c r="P180" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q180" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="181" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A181" t="s">
+        <v>200</v>
+      </c>
+      <c r="B181" t="s">
+        <v>192</v>
+      </c>
+      <c r="C181" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D181" t="s">
+        <v>69</v>
+      </c>
+      <c r="E181" t="s">
+        <v>201</v>
+      </c>
+      <c r="F181" t="s">
+        <v>36</v>
+      </c>
+      <c r="G181" t="s">
+        <v>197</v>
+      </c>
+      <c r="H181">
+        <v>14</v>
+      </c>
+      <c r="I181" t="s">
+        <v>8</v>
+      </c>
+      <c r="J181" t="s">
+        <v>45</v>
+      </c>
+      <c r="K181" t="s">
+        <v>198</v>
+      </c>
+      <c r="L181" s="14">
+        <v>517.70000000000005</v>
+      </c>
+      <c r="M181" s="15"/>
+      <c r="N181" s="14">
+        <v>407.4</v>
+      </c>
+      <c r="O181">
+        <v>657.9</v>
+      </c>
+      <c r="P181" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q181" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="182" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A182" t="s">
+        <v>200</v>
+      </c>
+      <c r="B182" t="s">
+        <v>192</v>
+      </c>
+      <c r="C182" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D182" t="s">
+        <v>69</v>
+      </c>
+      <c r="E182" t="s">
+        <v>201</v>
+      </c>
+      <c r="F182" t="s">
+        <v>36</v>
+      </c>
+      <c r="G182" t="s">
+        <v>197</v>
+      </c>
+      <c r="H182">
+        <v>42</v>
+      </c>
+      <c r="I182" t="s">
+        <v>8</v>
+      </c>
+      <c r="J182" t="s">
+        <v>45</v>
+      </c>
+      <c r="K182" t="s">
+        <v>198</v>
+      </c>
+      <c r="L182" s="14">
+        <v>300.5</v>
+      </c>
+      <c r="M182" s="15"/>
+      <c r="N182" s="14">
+        <v>251.7</v>
+      </c>
+      <c r="O182">
+        <v>358.6</v>
+      </c>
+      <c r="P182" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q182" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="183" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A183" t="s">
+        <v>200</v>
+      </c>
+      <c r="B183" t="s">
+        <v>192</v>
+      </c>
+      <c r="C183" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D183" t="s">
+        <v>69</v>
+      </c>
+      <c r="E183" t="s">
+        <v>201</v>
+      </c>
+      <c r="F183" t="s">
+        <v>36</v>
+      </c>
+      <c r="G183" t="s">
+        <v>197</v>
+      </c>
+      <c r="H183">
+        <v>42</v>
+      </c>
+      <c r="I183" t="s">
+        <v>8</v>
+      </c>
+      <c r="J183" t="s">
+        <v>45</v>
+      </c>
+      <c r="K183" t="s">
+        <v>198</v>
+      </c>
+      <c r="L183" s="14">
+        <v>506.1</v>
+      </c>
+      <c r="M183" s="15"/>
+      <c r="N183" s="14">
+        <v>395</v>
+      </c>
+      <c r="O183">
+        <v>648.4</v>
+      </c>
+      <c r="P183" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q183" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="184" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A184" t="s">
+        <v>200</v>
+      </c>
+      <c r="B184" t="s">
+        <v>192</v>
+      </c>
+      <c r="C184" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D184" t="s">
+        <v>69</v>
+      </c>
+      <c r="E184" t="s">
+        <v>201</v>
+      </c>
+      <c r="F184" t="s">
+        <v>36</v>
+      </c>
+      <c r="G184" t="s">
+        <v>197</v>
+      </c>
+      <c r="H184">
+        <v>210</v>
+      </c>
+      <c r="I184" t="s">
+        <v>8</v>
+      </c>
+      <c r="J184" t="s">
+        <v>45</v>
+      </c>
+      <c r="K184" t="s">
+        <v>198</v>
+      </c>
+      <c r="L184" s="14">
+        <v>244</v>
+      </c>
+      <c r="M184" s="15"/>
+      <c r="N184" s="14">
+        <v>202.6</v>
+      </c>
+      <c r="O184">
+        <v>293.7</v>
+      </c>
+      <c r="P184" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q184" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="185" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A185" t="s">
+        <v>200</v>
+      </c>
+      <c r="B185" t="s">
+        <v>192</v>
+      </c>
+      <c r="C185" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D185" t="s">
+        <v>69</v>
+      </c>
+      <c r="E185" t="s">
+        <v>201</v>
+      </c>
+      <c r="F185" t="s">
+        <v>36</v>
+      </c>
+      <c r="G185" t="s">
+        <v>197</v>
+      </c>
+      <c r="H185">
+        <v>210</v>
+      </c>
+      <c r="I185" t="s">
+        <v>8</v>
+      </c>
+      <c r="J185" t="s">
+        <v>45</v>
+      </c>
+      <c r="K185" t="s">
+        <v>198</v>
+      </c>
+      <c r="L185" s="14">
+        <v>570.6</v>
+      </c>
+      <c r="M185" s="15"/>
+      <c r="N185" s="14">
+        <v>453.7</v>
+      </c>
+      <c r="O185">
+        <v>717.6</v>
+      </c>
+      <c r="P185" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q185" s="13">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="186" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A186" t="s">
+        <v>200</v>
+      </c>
+      <c r="B186" t="s">
+        <v>192</v>
+      </c>
+      <c r="C186" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D186" t="s">
+        <v>69</v>
+      </c>
+      <c r="E186" t="s">
+        <v>202</v>
+      </c>
+      <c r="F186" t="s">
+        <v>36</v>
+      </c>
+      <c r="G186" t="s">
+        <v>197</v>
+      </c>
+      <c r="H186">
+        <v>0</v>
+      </c>
+      <c r="I186" t="s">
+        <v>8</v>
+      </c>
+      <c r="J186" t="s">
+        <v>45</v>
+      </c>
+      <c r="K186" t="s">
+        <v>198</v>
+      </c>
+      <c r="L186" s="14">
+        <v>208</v>
+      </c>
+      <c r="M186" s="15"/>
+      <c r="N186" s="14">
+        <v>180</v>
+      </c>
+      <c r="O186">
+        <v>240.3</v>
+      </c>
+      <c r="P186" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q186" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="187" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A187" t="s">
+        <v>200</v>
+      </c>
+      <c r="B187" t="s">
+        <v>192</v>
+      </c>
+      <c r="C187" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D187" t="s">
+        <v>69</v>
+      </c>
+      <c r="E187" t="s">
+        <v>202</v>
+      </c>
+      <c r="F187" t="s">
+        <v>36</v>
+      </c>
+      <c r="G187" t="s">
+        <v>197</v>
+      </c>
+      <c r="H187">
+        <v>0</v>
+      </c>
+      <c r="I187" t="s">
+        <v>8</v>
+      </c>
+      <c r="J187" t="s">
+        <v>45</v>
+      </c>
+      <c r="K187" t="s">
+        <v>198</v>
+      </c>
+      <c r="L187" s="14">
+        <v>364.9</v>
+      </c>
+      <c r="M187" s="15"/>
+      <c r="N187" s="14">
+        <v>285.60000000000002</v>
+      </c>
+      <c r="O187">
+        <v>466.2</v>
+      </c>
+      <c r="P187" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q187" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="188" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A188" t="s">
+        <v>200</v>
+      </c>
+      <c r="B188" t="s">
+        <v>192</v>
+      </c>
+      <c r="C188" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D188" t="s">
+        <v>69</v>
+      </c>
+      <c r="E188" t="s">
+        <v>202</v>
+      </c>
+      <c r="F188" t="s">
+        <v>36</v>
+      </c>
+      <c r="G188" t="s">
+        <v>197</v>
+      </c>
+      <c r="H188">
+        <v>14</v>
+      </c>
+      <c r="I188" t="s">
+        <v>8</v>
+      </c>
+      <c r="J188" t="s">
+        <v>45</v>
+      </c>
+      <c r="K188" t="s">
+        <v>198</v>
+      </c>
+      <c r="L188" s="14">
+        <v>259.8</v>
+      </c>
+      <c r="M188" s="15"/>
+      <c r="N188" s="14">
+        <v>222.5</v>
+      </c>
+      <c r="O188">
+        <v>303.39999999999998</v>
+      </c>
+      <c r="P188" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q188" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="189" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A189" t="s">
+        <v>200</v>
+      </c>
+      <c r="B189" t="s">
+        <v>192</v>
+      </c>
+      <c r="C189" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D189" t="s">
+        <v>69</v>
+      </c>
+      <c r="E189" t="s">
+        <v>202</v>
+      </c>
+      <c r="F189" t="s">
+        <v>36</v>
+      </c>
+      <c r="G189" t="s">
+        <v>197</v>
+      </c>
+      <c r="H189">
+        <v>14</v>
+      </c>
+      <c r="I189" t="s">
+        <v>8</v>
+      </c>
+      <c r="J189" t="s">
+        <v>45</v>
+      </c>
+      <c r="K189" t="s">
+        <v>198</v>
+      </c>
+      <c r="L189" s="14">
+        <v>464.5</v>
+      </c>
+      <c r="M189" s="15"/>
+      <c r="N189" s="14">
+        <v>363.7</v>
+      </c>
+      <c r="O189">
+        <v>593.29999999999995</v>
+      </c>
+      <c r="P189" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q189" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="190" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A190" t="s">
+        <v>200</v>
+      </c>
+      <c r="B190" t="s">
+        <v>192</v>
+      </c>
+      <c r="C190" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D190" t="s">
+        <v>69</v>
+      </c>
+      <c r="E190" t="s">
+        <v>202</v>
+      </c>
+      <c r="F190" t="s">
+        <v>36</v>
+      </c>
+      <c r="G190" t="s">
+        <v>197</v>
+      </c>
+      <c r="H190">
+        <v>42</v>
+      </c>
+      <c r="I190" t="s">
+        <v>8</v>
+      </c>
+      <c r="J190" t="s">
+        <v>45</v>
+      </c>
+      <c r="K190" t="s">
+        <v>198</v>
+      </c>
+      <c r="L190" s="14">
+        <v>278.89999999999998</v>
+      </c>
+      <c r="M190" s="15"/>
+      <c r="N190" s="14">
+        <v>239.2</v>
+      </c>
+      <c r="O190">
+        <v>325.2</v>
+      </c>
+      <c r="P190" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q190" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="191" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A191" t="s">
+        <v>200</v>
+      </c>
+      <c r="B191" t="s">
+        <v>192</v>
+      </c>
+      <c r="C191" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D191" t="s">
+        <v>69</v>
+      </c>
+      <c r="E191" t="s">
+        <v>202</v>
+      </c>
+      <c r="F191" t="s">
+        <v>36</v>
+      </c>
+      <c r="G191" t="s">
+        <v>197</v>
+      </c>
+      <c r="H191">
+        <v>42</v>
+      </c>
+      <c r="I191" t="s">
+        <v>8</v>
+      </c>
+      <c r="J191" t="s">
+        <v>45</v>
+      </c>
+      <c r="K191" t="s">
+        <v>198</v>
+      </c>
+      <c r="L191" s="14">
+        <v>507.4</v>
+      </c>
+      <c r="M191" s="15"/>
+      <c r="N191" s="14">
+        <v>396.4</v>
+      </c>
+      <c r="O191">
+        <v>649.6</v>
+      </c>
+      <c r="P191" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q191" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="192" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A192" t="s">
+        <v>200</v>
+      </c>
+      <c r="B192" t="s">
+        <v>192</v>
+      </c>
+      <c r="C192" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D192" t="s">
+        <v>69</v>
+      </c>
+      <c r="E192" t="s">
+        <v>202</v>
+      </c>
+      <c r="F192" t="s">
+        <v>36</v>
+      </c>
+      <c r="G192" t="s">
+        <v>197</v>
+      </c>
+      <c r="H192">
+        <v>210</v>
+      </c>
+      <c r="I192" t="s">
+        <v>8</v>
+      </c>
+      <c r="J192" t="s">
+        <v>45</v>
+      </c>
+      <c r="K192" t="s">
+        <v>198</v>
+      </c>
+      <c r="L192" s="14">
+        <v>205.4</v>
+      </c>
+      <c r="M192" s="15"/>
+      <c r="N192" s="14">
+        <v>175.5</v>
+      </c>
+      <c r="O192">
+        <v>240.5</v>
+      </c>
+      <c r="P192" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q192" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="193" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A193" t="s">
+        <v>200</v>
+      </c>
+      <c r="B193" t="s">
+        <v>192</v>
+      </c>
+      <c r="C193" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D193" t="s">
+        <v>69</v>
+      </c>
+      <c r="E193" t="s">
+        <v>202</v>
+      </c>
+      <c r="F193" t="s">
+        <v>36</v>
+      </c>
+      <c r="G193" t="s">
+        <v>197</v>
+      </c>
+      <c r="H193">
+        <v>210</v>
+      </c>
+      <c r="I193" t="s">
+        <v>8</v>
+      </c>
+      <c r="J193" t="s">
+        <v>45</v>
+      </c>
+      <c r="K193" t="s">
+        <v>198</v>
+      </c>
+      <c r="L193" s="14">
+        <v>458.1</v>
+      </c>
+      <c r="M193" s="15"/>
+      <c r="N193" s="14">
+        <v>361.9</v>
+      </c>
+      <c r="O193">
+        <v>579.79999999999995</v>
+      </c>
+      <c r="P193" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q193" s="13">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="194" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A194" t="s">
+        <v>200</v>
+      </c>
+      <c r="B194" t="s">
+        <v>192</v>
+      </c>
+      <c r="C194" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D194" t="s">
+        <v>69</v>
+      </c>
+      <c r="E194" t="s">
+        <v>203</v>
+      </c>
+      <c r="F194" t="s">
+        <v>36</v>
+      </c>
+      <c r="G194" t="s">
+        <v>197</v>
+      </c>
+      <c r="H194">
+        <v>0</v>
+      </c>
+      <c r="I194" t="s">
+        <v>8</v>
+      </c>
+      <c r="J194" t="s">
+        <v>45</v>
+      </c>
+      <c r="K194" t="s">
+        <v>199</v>
+      </c>
+      <c r="L194" s="14">
+        <v>234.9</v>
+      </c>
+      <c r="M194" s="15"/>
+      <c r="N194" s="14">
+        <v>200.4</v>
+      </c>
+      <c r="O194">
+        <v>275.3</v>
+      </c>
+      <c r="P194" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q194" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="195" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A195" t="s">
+        <v>200</v>
+      </c>
+      <c r="B195" t="s">
+        <v>192</v>
+      </c>
+      <c r="C195" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D195" t="s">
+        <v>69</v>
+      </c>
+      <c r="E195" t="s">
+        <v>203</v>
+      </c>
+      <c r="F195" t="s">
+        <v>36</v>
+      </c>
+      <c r="G195" t="s">
+        <v>197</v>
+      </c>
+      <c r="H195">
+        <v>0</v>
+      </c>
+      <c r="I195" t="s">
+        <v>8</v>
+      </c>
+      <c r="J195" t="s">
+        <v>45</v>
+      </c>
+      <c r="K195" t="s">
+        <v>199</v>
+      </c>
+      <c r="L195" s="14">
+        <v>426.9</v>
+      </c>
+      <c r="M195" s="15"/>
+      <c r="N195" s="14">
+        <v>331.7</v>
+      </c>
+      <c r="O195">
+        <v>549.4</v>
+      </c>
+      <c r="P195" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q195" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="196" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A196" t="s">
+        <v>200</v>
+      </c>
+      <c r="B196" t="s">
+        <v>192</v>
+      </c>
+      <c r="C196" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D196" t="s">
+        <v>69</v>
+      </c>
+      <c r="E196" t="s">
+        <v>203</v>
+      </c>
+      <c r="F196" t="s">
+        <v>36</v>
+      </c>
+      <c r="G196" t="s">
+        <v>197</v>
+      </c>
+      <c r="H196">
+        <v>14</v>
+      </c>
+      <c r="I196" t="s">
+        <v>8</v>
+      </c>
+      <c r="J196" t="s">
+        <v>45</v>
+      </c>
+      <c r="K196" t="s">
+        <v>199</v>
+      </c>
+      <c r="L196" s="14">
+        <v>356.9</v>
+      </c>
+      <c r="M196" s="15"/>
+      <c r="N196" s="14">
+        <v>298.8</v>
+      </c>
+      <c r="O196">
+        <v>426.4</v>
+      </c>
+      <c r="P196" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q196" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="197" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A197" t="s">
+        <v>200</v>
+      </c>
+      <c r="B197" t="s">
+        <v>192</v>
+      </c>
+      <c r="C197" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D197" t="s">
+        <v>69</v>
+      </c>
+      <c r="E197" t="s">
+        <v>203</v>
+      </c>
+      <c r="F197" t="s">
+        <v>36</v>
+      </c>
+      <c r="G197" t="s">
+        <v>197</v>
+      </c>
+      <c r="H197">
+        <v>14</v>
+      </c>
+      <c r="I197" t="s">
+        <v>8</v>
+      </c>
+      <c r="J197" t="s">
+        <v>45</v>
+      </c>
+      <c r="K197" t="s">
+        <v>199</v>
+      </c>
+      <c r="L197" s="14">
+        <v>688.6</v>
+      </c>
+      <c r="M197" s="15"/>
+      <c r="N197" s="14">
+        <v>528.6</v>
+      </c>
+      <c r="O197">
+        <v>896.9</v>
+      </c>
+      <c r="P197" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q197" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="198" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A198" t="s">
+        <v>200</v>
+      </c>
+      <c r="B198" t="s">
+        <v>192</v>
+      </c>
+      <c r="C198" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D198" t="s">
+        <v>69</v>
+      </c>
+      <c r="E198" t="s">
+        <v>203</v>
+      </c>
+      <c r="F198" t="s">
+        <v>36</v>
+      </c>
+      <c r="G198" t="s">
+        <v>197</v>
+      </c>
+      <c r="H198">
+        <v>42</v>
+      </c>
+      <c r="I198" t="s">
+        <v>8</v>
+      </c>
+      <c r="J198" t="s">
+        <v>45</v>
+      </c>
+      <c r="K198" t="s">
+        <v>199</v>
+      </c>
+      <c r="L198" s="14">
+        <v>311.89999999999998</v>
+      </c>
+      <c r="M198" s="15"/>
+      <c r="N198" s="14">
+        <v>261.7</v>
+      </c>
+      <c r="O198">
+        <v>371.7</v>
+      </c>
+      <c r="P198" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q198" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="199" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A199" t="s">
+        <v>200</v>
+      </c>
+      <c r="B199" t="s">
+        <v>192</v>
+      </c>
+      <c r="C199" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D199" t="s">
+        <v>69</v>
+      </c>
+      <c r="E199" t="s">
+        <v>203</v>
+      </c>
+      <c r="F199" t="s">
+        <v>36</v>
+      </c>
+      <c r="G199" t="s">
+        <v>197</v>
+      </c>
+      <c r="H199">
+        <v>42</v>
+      </c>
+      <c r="I199" t="s">
+        <v>8</v>
+      </c>
+      <c r="J199" t="s">
+        <v>45</v>
+      </c>
+      <c r="K199" t="s">
+        <v>199</v>
+      </c>
+      <c r="L199" s="14">
+        <v>615.1</v>
+      </c>
+      <c r="M199" s="15"/>
+      <c r="N199" s="14">
+        <v>468.9</v>
+      </c>
+      <c r="O199">
+        <v>806.8</v>
+      </c>
+      <c r="P199" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q199" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="200" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A200" t="s">
+        <v>200</v>
+      </c>
+      <c r="B200" t="s">
+        <v>192</v>
+      </c>
+      <c r="C200" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D200" t="s">
+        <v>69</v>
+      </c>
+      <c r="E200" t="s">
+        <v>203</v>
+      </c>
+      <c r="F200" t="s">
+        <v>36</v>
+      </c>
+      <c r="G200" t="s">
+        <v>197</v>
+      </c>
+      <c r="H200">
+        <v>210</v>
+      </c>
+      <c r="I200" t="s">
+        <v>8</v>
+      </c>
+      <c r="J200" t="s">
+        <v>45</v>
+      </c>
+      <c r="K200" t="s">
+        <v>199</v>
+      </c>
+      <c r="L200" s="14">
+        <v>228.2</v>
+      </c>
+      <c r="M200" s="15"/>
+      <c r="N200" s="14">
+        <v>193.8</v>
+      </c>
+      <c r="O200">
+        <v>268.5</v>
+      </c>
+      <c r="P200" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q200" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="201" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A201" t="s">
+        <v>200</v>
+      </c>
+      <c r="B201" t="s">
+        <v>192</v>
+      </c>
+      <c r="C201" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D201" t="s">
+        <v>69</v>
+      </c>
+      <c r="E201" t="s">
+        <v>203</v>
+      </c>
+      <c r="F201" t="s">
+        <v>36</v>
+      </c>
+      <c r="G201" t="s">
+        <v>197</v>
+      </c>
+      <c r="H201">
+        <v>210</v>
+      </c>
+      <c r="I201" t="s">
+        <v>8</v>
+      </c>
+      <c r="J201" t="s">
+        <v>45</v>
+      </c>
+      <c r="K201" t="s">
+        <v>199</v>
+      </c>
+      <c r="L201" s="14">
+        <v>606.1</v>
+      </c>
+      <c r="M201" s="15"/>
+      <c r="N201" s="14">
+        <v>479.9</v>
+      </c>
+      <c r="O201">
+        <v>765.3</v>
+      </c>
+      <c r="P201" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q201" s="13">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="202" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A202" t="s">
+        <v>200</v>
+      </c>
+      <c r="B202" t="s">
+        <v>192</v>
+      </c>
+      <c r="C202" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D202" t="s">
+        <v>69</v>
+      </c>
+      <c r="E202" t="s">
+        <v>204</v>
+      </c>
+      <c r="F202" t="s">
+        <v>36</v>
+      </c>
+      <c r="G202" t="s">
+        <v>197</v>
+      </c>
+      <c r="H202">
+        <v>0</v>
+      </c>
+      <c r="I202" t="s">
+        <v>8</v>
+      </c>
+      <c r="J202" t="s">
+        <v>45</v>
+      </c>
+      <c r="K202" t="s">
+        <v>199</v>
+      </c>
+      <c r="L202" s="15">
+        <v>276.39999999999998</v>
+      </c>
+      <c r="M202" s="15"/>
+      <c r="N202" s="15">
+        <v>235.9</v>
+      </c>
+      <c r="O202">
+        <v>323.89999999999998</v>
+      </c>
+      <c r="P202" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q202">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="203" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A203" t="s">
+        <v>200</v>
+      </c>
+      <c r="B203" t="s">
+        <v>192</v>
+      </c>
+      <c r="C203" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D203" t="s">
+        <v>69</v>
+      </c>
+      <c r="E203" t="s">
+        <v>204</v>
+      </c>
+      <c r="F203" t="s">
+        <v>36</v>
+      </c>
+      <c r="G203" t="s">
+        <v>197</v>
+      </c>
+      <c r="H203">
+        <v>0</v>
+      </c>
+      <c r="I203" t="s">
+        <v>8</v>
+      </c>
+      <c r="J203" t="s">
+        <v>45</v>
+      </c>
+      <c r="K203" t="s">
+        <v>199</v>
+      </c>
+      <c r="L203" s="15">
+        <v>498.6</v>
+      </c>
+      <c r="M203" s="15"/>
+      <c r="N203" s="15">
+        <v>395.6</v>
+      </c>
+      <c r="O203">
+        <v>628.5</v>
+      </c>
+      <c r="P203" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q203">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="204" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A204" t="s">
+        <v>200</v>
+      </c>
+      <c r="B204" t="s">
+        <v>192</v>
+      </c>
+      <c r="C204" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D204" t="s">
+        <v>69</v>
+      </c>
+      <c r="E204" t="s">
+        <v>204</v>
+      </c>
+      <c r="F204" t="s">
+        <v>36</v>
+      </c>
+      <c r="G204" t="s">
+        <v>197</v>
+      </c>
+      <c r="H204">
+        <v>14</v>
+      </c>
+      <c r="I204" t="s">
+        <v>8</v>
+      </c>
+      <c r="J204" t="s">
+        <v>45</v>
+      </c>
+      <c r="K204" t="s">
+        <v>199</v>
+      </c>
+      <c r="L204" s="15">
+        <v>398.8</v>
+      </c>
+      <c r="M204" s="15"/>
+      <c r="N204" s="15">
+        <v>340.8</v>
+      </c>
+      <c r="O204">
+        <v>466.6</v>
+      </c>
+      <c r="P204" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q204">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="205" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A205" t="s">
+        <v>200</v>
+      </c>
+      <c r="B205" t="s">
+        <v>192</v>
+      </c>
+      <c r="C205" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D205" t="s">
+        <v>69</v>
+      </c>
+      <c r="E205" t="s">
+        <v>204</v>
+      </c>
+      <c r="F205" t="s">
+        <v>36</v>
+      </c>
+      <c r="G205" t="s">
+        <v>197</v>
+      </c>
+      <c r="H205">
+        <v>14</v>
+      </c>
+      <c r="I205" t="s">
+        <v>8</v>
+      </c>
+      <c r="J205" t="s">
+        <v>45</v>
+      </c>
+      <c r="K205" t="s">
+        <v>199</v>
+      </c>
+      <c r="L205" s="15">
+        <v>638.20000000000005</v>
+      </c>
+      <c r="M205" s="15"/>
+      <c r="N205" s="15">
+        <v>510.9</v>
+      </c>
+      <c r="O205">
+        <v>797.3</v>
+      </c>
+      <c r="P205" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q205">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="206" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A206" t="s">
+        <v>200</v>
+      </c>
+      <c r="B206" t="s">
+        <v>192</v>
+      </c>
+      <c r="C206" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D206" t="s">
+        <v>69</v>
+      </c>
+      <c r="E206" t="s">
+        <v>204</v>
+      </c>
+      <c r="F206" t="s">
+        <v>36</v>
+      </c>
+      <c r="G206" t="s">
+        <v>197</v>
+      </c>
+      <c r="H206">
+        <v>42</v>
+      </c>
+      <c r="I206" t="s">
+        <v>8</v>
+      </c>
+      <c r="J206" t="s">
+        <v>45</v>
+      </c>
+      <c r="K206" t="s">
+        <v>199</v>
+      </c>
+      <c r="L206" s="15">
+        <v>373.3</v>
+      </c>
+      <c r="M206" s="15"/>
+      <c r="N206" s="15">
+        <v>320.89999999999998</v>
+      </c>
+      <c r="O206">
+        <v>434.2</v>
+      </c>
+      <c r="P206" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q206">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="207" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A207" t="s">
+        <v>200</v>
+      </c>
+      <c r="B207" t="s">
+        <v>192</v>
+      </c>
+      <c r="C207" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D207" t="s">
+        <v>69</v>
+      </c>
+      <c r="E207" t="s">
+        <v>204</v>
+      </c>
+      <c r="F207" t="s">
+        <v>36</v>
+      </c>
+      <c r="G207" t="s">
+        <v>197</v>
+      </c>
+      <c r="H207">
+        <v>42</v>
+      </c>
+      <c r="I207" t="s">
+        <v>8</v>
+      </c>
+      <c r="J207" t="s">
+        <v>45</v>
+      </c>
+      <c r="K207" t="s">
+        <v>199</v>
+      </c>
+      <c r="L207" s="15">
+        <v>674.3</v>
+      </c>
+      <c r="M207" s="15"/>
+      <c r="N207" s="15">
+        <v>544.9</v>
+      </c>
+      <c r="O207">
+        <v>834.4</v>
+      </c>
+      <c r="P207" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q207">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="208" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A208" t="s">
+        <v>200</v>
+      </c>
+      <c r="B208" t="s">
+        <v>192</v>
+      </c>
+      <c r="C208" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D208" t="s">
+        <v>69</v>
+      </c>
+      <c r="E208" t="s">
+        <v>204</v>
+      </c>
+      <c r="F208" t="s">
+        <v>36</v>
+      </c>
+      <c r="G208" t="s">
+        <v>197</v>
+      </c>
+      <c r="H208">
+        <v>210</v>
+      </c>
+      <c r="I208" t="s">
+        <v>8</v>
+      </c>
+      <c r="J208" t="s">
+        <v>45</v>
+      </c>
+      <c r="K208" t="s">
+        <v>199</v>
+      </c>
+      <c r="L208" s="15">
+        <v>266.7</v>
+      </c>
+      <c r="M208" s="15"/>
+      <c r="N208" s="15">
+        <v>228.6</v>
+      </c>
+      <c r="O208">
+        <v>311.10000000000002</v>
+      </c>
+      <c r="P208" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q208">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="209" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>200</v>
+      </c>
+      <c r="B209" t="s">
+        <v>192</v>
+      </c>
+      <c r="C209" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D209" t="s">
+        <v>69</v>
+      </c>
+      <c r="E209" t="s">
+        <v>204</v>
+      </c>
+      <c r="F209" t="s">
+        <v>36</v>
+      </c>
+      <c r="G209" t="s">
+        <v>197</v>
+      </c>
+      <c r="H209">
+        <v>210</v>
+      </c>
+      <c r="I209" t="s">
+        <v>8</v>
+      </c>
+      <c r="J209" t="s">
+        <v>45</v>
+      </c>
+      <c r="K209" t="s">
+        <v>199</v>
+      </c>
+      <c r="L209" s="15">
+        <v>583.20000000000005</v>
+      </c>
+      <c r="M209" s="15"/>
+      <c r="N209" s="15">
+        <v>471.2</v>
+      </c>
+      <c r="O209">
+        <v>721.9</v>
+      </c>
+      <c r="P209" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q209">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="210" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>200</v>
+      </c>
+      <c r="B210" t="s">
+        <v>192</v>
+      </c>
+      <c r="C210" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D210" t="s">
+        <v>69</v>
+      </c>
+      <c r="E210" t="s">
+        <v>201</v>
+      </c>
+      <c r="F210" t="s">
+        <v>36</v>
+      </c>
+      <c r="G210" t="s">
+        <v>197</v>
+      </c>
+      <c r="H210">
+        <v>0</v>
+      </c>
+      <c r="I210" t="s">
+        <v>8</v>
+      </c>
+      <c r="J210" t="s">
+        <v>16</v>
+      </c>
+      <c r="L210" s="15">
+        <v>251.7</v>
+      </c>
+      <c r="M210" s="15"/>
+      <c r="N210" s="15">
+        <v>213.7</v>
+      </c>
+      <c r="O210">
+        <v>296.60000000000002</v>
+      </c>
+      <c r="P210" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q210">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="211" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>200</v>
+      </c>
+      <c r="B211" t="s">
+        <v>192</v>
+      </c>
+      <c r="C211" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D211" t="s">
+        <v>69</v>
+      </c>
+      <c r="E211" t="s">
+        <v>201</v>
+      </c>
+      <c r="F211" t="s">
+        <v>36</v>
+      </c>
+      <c r="G211" t="s">
+        <v>197</v>
+      </c>
+      <c r="H211">
+        <v>0</v>
+      </c>
+      <c r="I211" t="s">
+        <v>8</v>
+      </c>
+      <c r="J211" t="s">
+        <v>16</v>
+      </c>
+      <c r="L211" s="15">
+        <v>477.5</v>
+      </c>
+      <c r="M211" s="15"/>
+      <c r="N211" s="15">
+        <v>361.3</v>
+      </c>
+      <c r="O211">
+        <v>630.9</v>
+      </c>
+      <c r="P211" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q211">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="212" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>200</v>
+      </c>
+      <c r="B212" t="s">
+        <v>192</v>
+      </c>
+      <c r="C212" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D212" t="s">
+        <v>69</v>
+      </c>
+      <c r="E212" t="s">
+        <v>201</v>
+      </c>
+      <c r="F212" t="s">
+        <v>36</v>
+      </c>
+      <c r="G212" t="s">
+        <v>197</v>
+      </c>
+      <c r="H212">
+        <v>14</v>
+      </c>
+      <c r="I212" t="s">
+        <v>8</v>
+      </c>
+      <c r="J212" t="s">
+        <v>16</v>
+      </c>
+      <c r="L212" s="15">
+        <v>235</v>
+      </c>
+      <c r="M212" s="15"/>
+      <c r="N212" s="15">
+        <v>202.1</v>
+      </c>
+      <c r="O212">
+        <v>273.2</v>
+      </c>
+      <c r="P212" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q212">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="213" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>200</v>
+      </c>
+      <c r="B213" t="s">
+        <v>192</v>
+      </c>
+      <c r="C213" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D213" t="s">
+        <v>69</v>
+      </c>
+      <c r="E213" t="s">
+        <v>201</v>
+      </c>
+      <c r="F213" t="s">
+        <v>36</v>
+      </c>
+      <c r="G213" t="s">
+        <v>197</v>
+      </c>
+      <c r="H213">
+        <v>14</v>
+      </c>
+      <c r="I213" t="s">
+        <v>8</v>
+      </c>
+      <c r="J213" t="s">
+        <v>16</v>
+      </c>
+      <c r="L213" s="15">
+        <v>441.4</v>
+      </c>
+      <c r="M213" s="15"/>
+      <c r="N213" s="15">
+        <v>331.6</v>
+      </c>
+      <c r="O213">
+        <v>587.6</v>
+      </c>
+      <c r="P213" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q213">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="214" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>200</v>
+      </c>
+      <c r="B214" t="s">
+        <v>192</v>
+      </c>
+      <c r="C214" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D214" t="s">
+        <v>69</v>
+      </c>
+      <c r="E214" t="s">
+        <v>201</v>
+      </c>
+      <c r="F214" t="s">
+        <v>36</v>
+      </c>
+      <c r="G214" t="s">
+        <v>197</v>
+      </c>
+      <c r="H214">
+        <v>42</v>
+      </c>
+      <c r="I214" t="s">
+        <v>8</v>
+      </c>
+      <c r="J214" t="s">
+        <v>16</v>
+      </c>
+      <c r="L214" s="15">
+        <v>229.3</v>
+      </c>
+      <c r="M214" s="15"/>
+      <c r="N214" s="15">
+        <v>195.2</v>
+      </c>
+      <c r="O214">
+        <v>269.39999999999998</v>
+      </c>
+      <c r="P214" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q214">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="215" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>200</v>
+      </c>
+      <c r="B215" t="s">
+        <v>192</v>
+      </c>
+      <c r="C215" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D215" t="s">
+        <v>69</v>
+      </c>
+      <c r="E215" t="s">
+        <v>201</v>
+      </c>
+      <c r="F215" t="s">
+        <v>36</v>
+      </c>
+      <c r="G215" t="s">
+        <v>197</v>
+      </c>
+      <c r="H215">
+        <v>42</v>
+      </c>
+      <c r="I215" t="s">
+        <v>8</v>
+      </c>
+      <c r="J215" t="s">
+        <v>16</v>
+      </c>
+      <c r="L215" s="15">
+        <v>454</v>
+      </c>
+      <c r="M215" s="15"/>
+      <c r="N215" s="15">
+        <v>340.7</v>
+      </c>
+      <c r="O215">
+        <v>605</v>
+      </c>
+      <c r="P215" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q215">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="216" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>200</v>
+      </c>
+      <c r="B216" t="s">
+        <v>192</v>
+      </c>
+      <c r="C216" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D216" t="s">
+        <v>69</v>
+      </c>
+      <c r="E216" t="s">
+        <v>201</v>
+      </c>
+      <c r="F216" t="s">
+        <v>36</v>
+      </c>
+      <c r="G216" t="s">
+        <v>197</v>
+      </c>
+      <c r="H216">
+        <v>210</v>
+      </c>
+      <c r="I216" t="s">
+        <v>8</v>
+      </c>
+      <c r="J216" t="s">
+        <v>16</v>
+      </c>
+      <c r="L216" s="15">
+        <v>202.2</v>
+      </c>
+      <c r="M216" s="15"/>
+      <c r="N216" s="15">
+        <v>172.4</v>
+      </c>
+      <c r="O216">
+        <v>237.1</v>
+      </c>
+      <c r="P216" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q216">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="217" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>200</v>
+      </c>
+      <c r="B217" t="s">
+        <v>192</v>
+      </c>
+      <c r="C217" t="str">
+        <f t="shared" si="22"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D217" t="s">
+        <v>69</v>
+      </c>
+      <c r="E217" t="s">
+        <v>201</v>
+      </c>
+      <c r="F217" t="s">
+        <v>36</v>
+      </c>
+      <c r="G217" t="s">
+        <v>197</v>
+      </c>
+      <c r="H217">
+        <v>210</v>
+      </c>
+      <c r="I217" t="s">
+        <v>8</v>
+      </c>
+      <c r="J217" t="s">
+        <v>16</v>
+      </c>
+      <c r="L217" s="15">
+        <v>518.1</v>
+      </c>
+      <c r="M217" s="15"/>
+      <c r="N217" s="15">
+        <v>398.7</v>
+      </c>
+      <c r="O217">
+        <v>673.3</v>
+      </c>
+      <c r="P217" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q217">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="218" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>200</v>
+      </c>
+      <c r="B218" t="s">
+        <v>192</v>
+      </c>
+      <c r="C218" t="str">
+        <f t="shared" ref="C218:C241" si="23">B218</f>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D218" t="s">
+        <v>69</v>
+      </c>
+      <c r="E218" t="s">
+        <v>202</v>
+      </c>
+      <c r="F218" t="s">
+        <v>36</v>
+      </c>
+      <c r="G218" t="s">
+        <v>197</v>
+      </c>
+      <c r="H218">
+        <v>0</v>
+      </c>
+      <c r="I218" t="s">
+        <v>8</v>
+      </c>
+      <c r="J218" t="s">
+        <v>16</v>
+      </c>
+      <c r="L218" s="15">
+        <v>251.7</v>
+      </c>
+      <c r="M218" s="15"/>
+      <c r="N218" s="15">
+        <v>213.7</v>
+      </c>
+      <c r="O218">
+        <v>296.60000000000002</v>
+      </c>
+      <c r="P218" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q218">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="219" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>200</v>
+      </c>
+      <c r="B219" t="s">
+        <v>192</v>
+      </c>
+      <c r="C219" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D219" t="s">
+        <v>69</v>
+      </c>
+      <c r="E219" t="s">
+        <v>202</v>
+      </c>
+      <c r="F219" t="s">
+        <v>36</v>
+      </c>
+      <c r="G219" t="s">
+        <v>197</v>
+      </c>
+      <c r="H219">
+        <v>0</v>
+      </c>
+      <c r="I219" t="s">
+        <v>8</v>
+      </c>
+      <c r="J219" t="s">
+        <v>16</v>
+      </c>
+      <c r="L219" s="15">
+        <v>477.5</v>
+      </c>
+      <c r="M219" s="15"/>
+      <c r="N219" s="15">
+        <v>361.3</v>
+      </c>
+      <c r="O219">
+        <v>630.9</v>
+      </c>
+      <c r="P219" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q219">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="220" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>200</v>
+      </c>
+      <c r="B220" t="s">
+        <v>192</v>
+      </c>
+      <c r="C220" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D220" t="s">
+        <v>69</v>
+      </c>
+      <c r="E220" t="s">
+        <v>202</v>
+      </c>
+      <c r="F220" t="s">
+        <v>36</v>
+      </c>
+      <c r="G220" t="s">
+        <v>197</v>
+      </c>
+      <c r="H220">
+        <v>14</v>
+      </c>
+      <c r="I220" t="s">
+        <v>8</v>
+      </c>
+      <c r="J220" t="s">
+        <v>16</v>
+      </c>
+      <c r="L220" s="15">
+        <v>235</v>
+      </c>
+      <c r="M220" s="15"/>
+      <c r="N220" s="15">
+        <v>202.1</v>
+      </c>
+      <c r="O220">
+        <v>273.2</v>
+      </c>
+      <c r="P220" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q220">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="221" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>200</v>
+      </c>
+      <c r="B221" t="s">
+        <v>192</v>
+      </c>
+      <c r="C221" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D221" t="s">
+        <v>69</v>
+      </c>
+      <c r="E221" t="s">
+        <v>202</v>
+      </c>
+      <c r="F221" t="s">
+        <v>36</v>
+      </c>
+      <c r="G221" t="s">
+        <v>197</v>
+      </c>
+      <c r="H221">
+        <v>14</v>
+      </c>
+      <c r="I221" t="s">
+        <v>8</v>
+      </c>
+      <c r="J221" t="s">
+        <v>16</v>
+      </c>
+      <c r="L221" s="15">
+        <v>441.4</v>
+      </c>
+      <c r="M221" s="15"/>
+      <c r="N221" s="15">
+        <v>331.6</v>
+      </c>
+      <c r="O221">
+        <v>587.6</v>
+      </c>
+      <c r="P221" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q221">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="222" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>200</v>
+      </c>
+      <c r="B222" t="s">
+        <v>192</v>
+      </c>
+      <c r="C222" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D222" t="s">
+        <v>69</v>
+      </c>
+      <c r="E222" t="s">
+        <v>202</v>
+      </c>
+      <c r="F222" t="s">
+        <v>36</v>
+      </c>
+      <c r="G222" t="s">
+        <v>197</v>
+      </c>
+      <c r="H222">
+        <v>42</v>
+      </c>
+      <c r="I222" t="s">
+        <v>8</v>
+      </c>
+      <c r="J222" t="s">
+        <v>16</v>
+      </c>
+      <c r="L222" s="15">
+        <v>229.3</v>
+      </c>
+      <c r="M222" s="15"/>
+      <c r="N222" s="15">
+        <v>195.2</v>
+      </c>
+      <c r="O222">
+        <v>269.39999999999998</v>
+      </c>
+      <c r="P222" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q222">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="223" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>200</v>
+      </c>
+      <c r="B223" t="s">
+        <v>192</v>
+      </c>
+      <c r="C223" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D223" t="s">
+        <v>69</v>
+      </c>
+      <c r="E223" t="s">
+        <v>202</v>
+      </c>
+      <c r="F223" t="s">
+        <v>36</v>
+      </c>
+      <c r="G223" t="s">
+        <v>197</v>
+      </c>
+      <c r="H223">
+        <v>42</v>
+      </c>
+      <c r="I223" t="s">
+        <v>8</v>
+      </c>
+      <c r="J223" t="s">
+        <v>16</v>
+      </c>
+      <c r="L223" s="15">
+        <v>454</v>
+      </c>
+      <c r="M223" s="15"/>
+      <c r="N223" s="15">
+        <v>340.7</v>
+      </c>
+      <c r="O223">
+        <v>605</v>
+      </c>
+      <c r="P223" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q223">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="224" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>200</v>
+      </c>
+      <c r="B224" t="s">
+        <v>192</v>
+      </c>
+      <c r="C224" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D224" t="s">
+        <v>69</v>
+      </c>
+      <c r="E224" t="s">
+        <v>202</v>
+      </c>
+      <c r="F224" t="s">
+        <v>36</v>
+      </c>
+      <c r="G224" t="s">
+        <v>197</v>
+      </c>
+      <c r="H224">
+        <v>210</v>
+      </c>
+      <c r="I224" t="s">
+        <v>8</v>
+      </c>
+      <c r="J224" t="s">
+        <v>16</v>
+      </c>
+      <c r="L224" s="15">
+        <v>202.2</v>
+      </c>
+      <c r="M224" s="15"/>
+      <c r="N224" s="15">
+        <v>172.4</v>
+      </c>
+      <c r="O224">
+        <v>237.1</v>
+      </c>
+      <c r="P224" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q224">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="225" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>200</v>
+      </c>
+      <c r="B225" t="s">
+        <v>192</v>
+      </c>
+      <c r="C225" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D225" t="s">
+        <v>69</v>
+      </c>
+      <c r="E225" t="s">
+        <v>202</v>
+      </c>
+      <c r="F225" t="s">
+        <v>36</v>
+      </c>
+      <c r="G225" t="s">
+        <v>197</v>
+      </c>
+      <c r="H225">
+        <v>210</v>
+      </c>
+      <c r="I225" t="s">
+        <v>8</v>
+      </c>
+      <c r="J225" t="s">
+        <v>16</v>
+      </c>
+      <c r="L225" s="15">
+        <v>518.1</v>
+      </c>
+      <c r="M225" s="15"/>
+      <c r="N225" s="15">
+        <v>398.7</v>
+      </c>
+      <c r="O225">
+        <v>673.3</v>
+      </c>
+      <c r="P225" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q225">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="226" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>200</v>
+      </c>
+      <c r="B226" t="s">
+        <v>192</v>
+      </c>
+      <c r="C226" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D226" t="s">
+        <v>69</v>
+      </c>
+      <c r="E226" t="s">
+        <v>203</v>
+      </c>
+      <c r="F226" t="s">
+        <v>36</v>
+      </c>
+      <c r="G226" t="s">
+        <v>197</v>
+      </c>
+      <c r="H226">
+        <v>0</v>
+      </c>
+      <c r="I226" t="s">
+        <v>8</v>
+      </c>
+      <c r="J226" t="s">
+        <v>16</v>
+      </c>
+      <c r="L226" s="15">
+        <v>251.7</v>
+      </c>
+      <c r="M226" s="15"/>
+      <c r="N226" s="15">
+        <v>213.7</v>
+      </c>
+      <c r="O226">
+        <v>296.60000000000002</v>
+      </c>
+      <c r="P226" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q226">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="227" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>200</v>
+      </c>
+      <c r="B227" t="s">
+        <v>192</v>
+      </c>
+      <c r="C227" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D227" t="s">
+        <v>69</v>
+      </c>
+      <c r="E227" t="s">
+        <v>203</v>
+      </c>
+      <c r="F227" t="s">
+        <v>36</v>
+      </c>
+      <c r="G227" t="s">
+        <v>197</v>
+      </c>
+      <c r="H227">
+        <v>0</v>
+      </c>
+      <c r="I227" t="s">
+        <v>8</v>
+      </c>
+      <c r="J227" t="s">
+        <v>16</v>
+      </c>
+      <c r="L227" s="15">
+        <v>477.5</v>
+      </c>
+      <c r="M227" s="15"/>
+      <c r="N227" s="15">
+        <v>361.3</v>
+      </c>
+      <c r="O227">
+        <v>630.9</v>
+      </c>
+      <c r="P227" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q227">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="228" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>200</v>
+      </c>
+      <c r="B228" t="s">
+        <v>192</v>
+      </c>
+      <c r="C228" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D228" t="s">
+        <v>69</v>
+      </c>
+      <c r="E228" t="s">
+        <v>203</v>
+      </c>
+      <c r="F228" t="s">
+        <v>36</v>
+      </c>
+      <c r="G228" t="s">
+        <v>197</v>
+      </c>
+      <c r="H228">
+        <v>14</v>
+      </c>
+      <c r="I228" t="s">
+        <v>8</v>
+      </c>
+      <c r="J228" t="s">
+        <v>16</v>
+      </c>
+      <c r="L228" s="15">
+        <v>235</v>
+      </c>
+      <c r="M228" s="15"/>
+      <c r="N228" s="15">
+        <v>202.1</v>
+      </c>
+      <c r="O228">
+        <v>273.2</v>
+      </c>
+      <c r="P228" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q228">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="229" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>200</v>
+      </c>
+      <c r="B229" t="s">
+        <v>192</v>
+      </c>
+      <c r="C229" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D229" t="s">
+        <v>69</v>
+      </c>
+      <c r="E229" t="s">
+        <v>203</v>
+      </c>
+      <c r="F229" t="s">
+        <v>36</v>
+      </c>
+      <c r="G229" t="s">
+        <v>197</v>
+      </c>
+      <c r="H229">
+        <v>14</v>
+      </c>
+      <c r="I229" t="s">
+        <v>8</v>
+      </c>
+      <c r="J229" t="s">
+        <v>16</v>
+      </c>
+      <c r="L229" s="15">
+        <v>441.4</v>
+      </c>
+      <c r="M229" s="15"/>
+      <c r="N229" s="15">
+        <v>331.6</v>
+      </c>
+      <c r="O229">
+        <v>587.6</v>
+      </c>
+      <c r="P229" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q229">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="230" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>200</v>
+      </c>
+      <c r="B230" t="s">
+        <v>192</v>
+      </c>
+      <c r="C230" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D230" t="s">
+        <v>69</v>
+      </c>
+      <c r="E230" t="s">
+        <v>203</v>
+      </c>
+      <c r="F230" t="s">
+        <v>36</v>
+      </c>
+      <c r="G230" t="s">
+        <v>197</v>
+      </c>
+      <c r="H230">
+        <v>42</v>
+      </c>
+      <c r="I230" t="s">
+        <v>8</v>
+      </c>
+      <c r="J230" t="s">
+        <v>16</v>
+      </c>
+      <c r="L230" s="15">
+        <v>229.3</v>
+      </c>
+      <c r="M230" s="15"/>
+      <c r="N230" s="15">
+        <v>195.2</v>
+      </c>
+      <c r="O230">
+        <v>269.39999999999998</v>
+      </c>
+      <c r="P230" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q230">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="231" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>200</v>
+      </c>
+      <c r="B231" t="s">
+        <v>192</v>
+      </c>
+      <c r="C231" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D231" t="s">
+        <v>69</v>
+      </c>
+      <c r="E231" t="s">
+        <v>203</v>
+      </c>
+      <c r="F231" t="s">
+        <v>36</v>
+      </c>
+      <c r="G231" t="s">
+        <v>197</v>
+      </c>
+      <c r="H231">
+        <v>42</v>
+      </c>
+      <c r="I231" t="s">
+        <v>8</v>
+      </c>
+      <c r="J231" t="s">
+        <v>16</v>
+      </c>
+      <c r="L231" s="15">
+        <v>454</v>
+      </c>
+      <c r="M231" s="15"/>
+      <c r="N231" s="15">
+        <v>340.7</v>
+      </c>
+      <c r="O231">
+        <v>605</v>
+      </c>
+      <c r="P231" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q231">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="232" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>200</v>
+      </c>
+      <c r="B232" t="s">
+        <v>192</v>
+      </c>
+      <c r="C232" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D232" t="s">
+        <v>69</v>
+      </c>
+      <c r="E232" t="s">
+        <v>203</v>
+      </c>
+      <c r="F232" t="s">
+        <v>36</v>
+      </c>
+      <c r="G232" t="s">
+        <v>197</v>
+      </c>
+      <c r="H232">
+        <v>210</v>
+      </c>
+      <c r="I232" t="s">
+        <v>8</v>
+      </c>
+      <c r="J232" t="s">
+        <v>16</v>
+      </c>
+      <c r="L232" s="15">
+        <v>202.2</v>
+      </c>
+      <c r="M232" s="15"/>
+      <c r="N232" s="15">
+        <v>172.4</v>
+      </c>
+      <c r="O232">
+        <v>237.1</v>
+      </c>
+      <c r="P232" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q232">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="233" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>200</v>
+      </c>
+      <c r="B233" t="s">
+        <v>192</v>
+      </c>
+      <c r="C233" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D233" t="s">
+        <v>69</v>
+      </c>
+      <c r="E233" t="s">
+        <v>203</v>
+      </c>
+      <c r="F233" t="s">
+        <v>36</v>
+      </c>
+      <c r="G233" t="s">
+        <v>197</v>
+      </c>
+      <c r="H233">
+        <v>210</v>
+      </c>
+      <c r="I233" t="s">
+        <v>8</v>
+      </c>
+      <c r="J233" t="s">
+        <v>16</v>
+      </c>
+      <c r="L233" s="15">
+        <v>518.1</v>
+      </c>
+      <c r="M233" s="15"/>
+      <c r="N233" s="15">
+        <v>398.7</v>
+      </c>
+      <c r="O233">
+        <v>673.3</v>
+      </c>
+      <c r="P233" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q233">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="234" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>200</v>
+      </c>
+      <c r="B234" t="s">
+        <v>192</v>
+      </c>
+      <c r="C234" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D234" t="s">
+        <v>69</v>
+      </c>
+      <c r="E234" t="s">
+        <v>204</v>
+      </c>
+      <c r="F234" t="s">
+        <v>36</v>
+      </c>
+      <c r="G234" t="s">
+        <v>197</v>
+      </c>
+      <c r="H234">
+        <v>0</v>
+      </c>
+      <c r="I234" t="s">
+        <v>8</v>
+      </c>
+      <c r="J234" t="s">
+        <v>16</v>
+      </c>
+      <c r="L234" s="15">
+        <v>251.7</v>
+      </c>
+      <c r="M234" s="15"/>
+      <c r="N234" s="15">
+        <v>213.7</v>
+      </c>
+      <c r="O234">
+        <v>296.60000000000002</v>
+      </c>
+      <c r="P234" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q234">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="235" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>200</v>
+      </c>
+      <c r="B235" t="s">
+        <v>192</v>
+      </c>
+      <c r="C235" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D235" t="s">
+        <v>69</v>
+      </c>
+      <c r="E235" t="s">
+        <v>204</v>
+      </c>
+      <c r="F235" t="s">
+        <v>36</v>
+      </c>
+      <c r="G235" t="s">
+        <v>197</v>
+      </c>
+      <c r="H235">
+        <v>0</v>
+      </c>
+      <c r="I235" t="s">
+        <v>8</v>
+      </c>
+      <c r="J235" t="s">
+        <v>16</v>
+      </c>
+      <c r="L235" s="15">
+        <v>477.5</v>
+      </c>
+      <c r="M235" s="15"/>
+      <c r="N235" s="15">
+        <v>361.3</v>
+      </c>
+      <c r="O235">
+        <v>630.9</v>
+      </c>
+      <c r="P235" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q235">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="236" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>200</v>
+      </c>
+      <c r="B236" t="s">
+        <v>192</v>
+      </c>
+      <c r="C236" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D236" t="s">
+        <v>69</v>
+      </c>
+      <c r="E236" t="s">
+        <v>204</v>
+      </c>
+      <c r="F236" t="s">
+        <v>36</v>
+      </c>
+      <c r="G236" t="s">
+        <v>197</v>
+      </c>
+      <c r="H236">
+        <v>14</v>
+      </c>
+      <c r="I236" t="s">
+        <v>8</v>
+      </c>
+      <c r="J236" t="s">
+        <v>16</v>
+      </c>
+      <c r="L236" s="15">
+        <v>235</v>
+      </c>
+      <c r="M236" s="15"/>
+      <c r="N236" s="15">
+        <v>202.1</v>
+      </c>
+      <c r="O236">
+        <v>273.2</v>
+      </c>
+      <c r="P236" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q236">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="237" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>200</v>
+      </c>
+      <c r="B237" t="s">
+        <v>192</v>
+      </c>
+      <c r="C237" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D237" t="s">
+        <v>69</v>
+      </c>
+      <c r="E237" t="s">
+        <v>204</v>
+      </c>
+      <c r="F237" t="s">
+        <v>36</v>
+      </c>
+      <c r="G237" t="s">
+        <v>197</v>
+      </c>
+      <c r="H237">
+        <v>14</v>
+      </c>
+      <c r="I237" t="s">
+        <v>8</v>
+      </c>
+      <c r="J237" t="s">
+        <v>16</v>
+      </c>
+      <c r="L237" s="15">
+        <v>441.4</v>
+      </c>
+      <c r="M237" s="15"/>
+      <c r="N237" s="15">
+        <v>331.6</v>
+      </c>
+      <c r="O237">
+        <v>587.6</v>
+      </c>
+      <c r="P237" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q237">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="238" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
+        <v>200</v>
+      </c>
+      <c r="B238" t="s">
+        <v>192</v>
+      </c>
+      <c r="C238" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D238" t="s">
+        <v>69</v>
+      </c>
+      <c r="E238" t="s">
+        <v>204</v>
+      </c>
+      <c r="F238" t="s">
+        <v>36</v>
+      </c>
+      <c r="G238" t="s">
+        <v>197</v>
+      </c>
+      <c r="H238">
+        <v>42</v>
+      </c>
+      <c r="I238" t="s">
+        <v>8</v>
+      </c>
+      <c r="J238" t="s">
+        <v>16</v>
+      </c>
+      <c r="L238" s="15">
+        <v>229.3</v>
+      </c>
+      <c r="M238" s="15"/>
+      <c r="N238" s="15">
+        <v>195.2</v>
+      </c>
+      <c r="O238">
+        <v>269.39999999999998</v>
+      </c>
+      <c r="P238" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q238">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="239" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>200</v>
+      </c>
+      <c r="B239" t="s">
+        <v>192</v>
+      </c>
+      <c r="C239" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D239" t="s">
+        <v>69</v>
+      </c>
+      <c r="E239" t="s">
+        <v>204</v>
+      </c>
+      <c r="F239" t="s">
+        <v>36</v>
+      </c>
+      <c r="G239" t="s">
+        <v>197</v>
+      </c>
+      <c r="H239">
+        <v>42</v>
+      </c>
+      <c r="I239" t="s">
+        <v>8</v>
+      </c>
+      <c r="J239" t="s">
+        <v>16</v>
+      </c>
+      <c r="L239" s="15">
+        <v>454</v>
+      </c>
+      <c r="M239" s="15"/>
+      <c r="N239" s="15">
+        <v>340.7</v>
+      </c>
+      <c r="O239">
+        <v>605</v>
+      </c>
+      <c r="P239" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q239">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="240" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A240" t="s">
+        <v>200</v>
+      </c>
+      <c r="B240" t="s">
+        <v>192</v>
+      </c>
+      <c r="C240" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D240" t="s">
+        <v>69</v>
+      </c>
+      <c r="E240" t="s">
+        <v>204</v>
+      </c>
+      <c r="F240" t="s">
+        <v>36</v>
+      </c>
+      <c r="G240" t="s">
+        <v>197</v>
+      </c>
+      <c r="H240">
+        <v>210</v>
+      </c>
+      <c r="I240" t="s">
+        <v>8</v>
+      </c>
+      <c r="J240" t="s">
+        <v>16</v>
+      </c>
+      <c r="L240" s="15">
+        <v>202.2</v>
+      </c>
+      <c r="M240" s="15"/>
+      <c r="N240" s="15">
+        <v>172.4</v>
+      </c>
+      <c r="O240">
+        <v>237.1</v>
+      </c>
+      <c r="P240" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q240">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="241" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A241" t="s">
+        <v>200</v>
+      </c>
+      <c r="B241" t="s">
+        <v>192</v>
+      </c>
+      <c r="C241" t="str">
+        <f t="shared" si="23"/>
+        <v>BavarianNordic</v>
+      </c>
+      <c r="D241" t="s">
+        <v>69</v>
+      </c>
+      <c r="E241" t="s">
+        <v>204</v>
+      </c>
+      <c r="F241" t="s">
+        <v>36</v>
+      </c>
+      <c r="G241" t="s">
+        <v>197</v>
+      </c>
+      <c r="H241">
+        <v>210</v>
+      </c>
+      <c r="I241" t="s">
+        <v>8</v>
+      </c>
+      <c r="J241" t="s">
+        <v>16</v>
+      </c>
+      <c r="L241" s="15">
+        <v>518.1</v>
+      </c>
+      <c r="M241" s="15"/>
+      <c r="N241" s="15">
+        <v>398.7</v>
+      </c>
+      <c r="O241">
+        <v>673.3</v>
+      </c>
+      <c r="P241" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q241">
+        <v>83</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:AH177" xr:uid="{FF8BCAD0-FE00-D14F-8109-AD4E81997C16}"/>
+  <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -11141,8 +14469,8 @@
   <dimension ref="A1:O65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A28" sqref="A28:XFD36"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12886,10 +16214,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B96E09-4BF7-5E4A-9A2D-7FF2A0B754F5}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -13054,122 +16382,122 @@
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="B9" s="9" t="s">
+      <c r="B9" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C9" s="9" t="s">
+      <c r="C9" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="F9" s="9" t="s">
+      <c r="F9" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="9" t="s">
+      <c r="G9" s="10"/>
+      <c r="H9" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="I9" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="J9" s="11" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E10" s="9" t="s">
+      <c r="E10" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="10" t="s">
         <v>92</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
-      <c r="I10" s="9" t="s">
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="J10" s="11" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="9" t="s">
+      <c r="A11" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="9" t="s">
+      <c r="C11" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D11" s="9" t="s">
+      <c r="D11" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F11" s="9" t="s">
+      <c r="F11" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="H11" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="I11" s="9" t="s">
+      <c r="I11" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="J11" s="11" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A12" s="9" t="s">
+      <c r="A12" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="B12" s="9" t="s">
+      <c r="B12" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C12" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="D12" s="9" t="s">
+      <c r="D12" s="10" t="s">
         <v>165</v>
       </c>
-      <c r="E12" s="9" t="s">
+      <c r="E12" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="9" t="s">
+      <c r="F12" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="10" t="s">
         <v>166</v>
       </c>
-      <c r="H12" s="9"/>
-      <c r="I12" s="9" t="s">
+      <c r="H12" s="10"/>
+      <c r="I12" s="10" t="s">
         <v>172</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="J12" s="11" t="s">
         <v>131</v>
       </c>
     </row>
@@ -13189,7 +16517,7 @@
       <c r="G13" t="s">
         <v>129</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="9" t="s">
         <v>128</v>
       </c>
     </row>
@@ -13205,6 +16533,105 @@
       </c>
       <c r="J14" t="s">
         <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>186</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>184</v>
+      </c>
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="G16" t="s">
+        <v>61</v>
+      </c>
+      <c r="J16" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>183</v>
+      </c>
+      <c r="G17" t="s">
+        <v>182</v>
+      </c>
+      <c r="J17" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>188</v>
+      </c>
+      <c r="B18" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" t="s">
+        <v>119</v>
+      </c>
+      <c r="J18" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C19" t="s">
+        <v>197</v>
+      </c>
+      <c r="E19" t="s">
+        <v>193</v>
+      </c>
+      <c r="F19" t="s">
+        <v>191</v>
+      </c>
+      <c r="G19" t="s">
+        <v>194</v>
+      </c>
+      <c r="J19" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" t="s">
+        <v>192</v>
+      </c>
+      <c r="C20" t="s">
+        <v>197</v>
+      </c>
+      <c r="E20" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>191</v>
+      </c>
+      <c r="J20" t="s">
+        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -13213,6 +16640,8 @@
     <hyperlink ref="J9" r:id="rId2" xr:uid="{F0CF3696-1BA1-5C43-9863-A926EBA2EA13}"/>
     <hyperlink ref="J10" r:id="rId3" xr:uid="{EAD1F518-105F-A543-A35F-D9623B74AF78}"/>
     <hyperlink ref="J12" r:id="rId4" xr:uid="{6E80B355-568F-5044-97B9-11158FDCBA4C}"/>
+    <hyperlink ref="J13" r:id="rId5" xr:uid="{36D6FECF-5061-174F-90CC-DB73E4F2E12F}"/>
+    <hyperlink ref="J18" r:id="rId6" xr:uid="{CC16F52F-6E02-5A48-8D89-9512EB3E6A27}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
include updated data and summary
</commit_message>
<xml_diff>
--- a/raw-data/RSV Data 2024.xlsx
+++ b/raw-data/RSV Data 2024.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deborah/github/RSVcorrelates/raw-data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/z2211982/github/RSVcorrelates/raw-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9896ABCC-5D01-0549-AA1A-789A3E0D27E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84B733E1-D8DC-6B47-8B63-AC60551E43D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6140" yWindow="1940" windowWidth="24780" windowHeight="18620" activeTab="2" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
+    <workbookView xWindow="6140" yWindow="1940" windowWidth="24780" windowHeight="18620" activeTab="3" xr2:uid="{EB31B1D0-F9A6-424A-A571-FCA1CB7357B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Antibodies" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2719" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2720" uniqueCount="206">
   <si>
     <t>Trial</t>
   </si>
@@ -658,6 +658,9 @@
   </si>
   <si>
     <t>high dose (+later dose)</t>
+  </si>
+  <si>
+    <t>Relationship of Serum Antibody to Risk of Respiratory Syncytial Virus Infection in Elderly Adults</t>
   </si>
 </sst>
 </file>
@@ -738,7 +741,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -757,7 +760,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1946,9 +1948,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1986,7 +1988,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2092,7 +2094,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2234,7 +2236,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9880,7 +9882,7 @@
       <c r="F150" t="s">
         <v>36</v>
       </c>
-      <c r="G150" s="12" t="s">
+      <c r="G150" t="s">
         <v>179</v>
       </c>
       <c r="H150">
@@ -9892,7 +9894,7 @@
       <c r="J150" t="s">
         <v>45</v>
       </c>
-      <c r="K150" s="12" t="s">
+      <c r="K150" t="s">
         <v>165</v>
       </c>
       <c r="L150">
@@ -9928,7 +9930,7 @@
       <c r="F151" t="s">
         <v>36</v>
       </c>
-      <c r="G151" s="12" t="s">
+      <c r="G151" t="s">
         <v>179</v>
       </c>
       <c r="H151">
@@ -9940,7 +9942,7 @@
       <c r="J151" t="s">
         <v>45</v>
       </c>
-      <c r="K151" s="12" t="s">
+      <c r="K151" t="s">
         <v>165</v>
       </c>
       <c r="L151">
@@ -9976,7 +9978,7 @@
       <c r="F152" t="s">
         <v>36</v>
       </c>
-      <c r="G152" s="12" t="s">
+      <c r="G152" t="s">
         <v>179</v>
       </c>
       <c r="H152">
@@ -9988,7 +9990,7 @@
       <c r="J152" t="s">
         <v>45</v>
       </c>
-      <c r="K152" s="12" t="s">
+      <c r="K152" t="s">
         <v>165</v>
       </c>
       <c r="L152">
@@ -10024,7 +10026,7 @@
       <c r="F153" t="s">
         <v>36</v>
       </c>
-      <c r="G153" s="12" t="s">
+      <c r="G153" t="s">
         <v>179</v>
       </c>
       <c r="H153">
@@ -10036,7 +10038,7 @@
       <c r="J153" t="s">
         <v>45</v>
       </c>
-      <c r="K153" s="12" t="s">
+      <c r="K153" t="s">
         <v>165</v>
       </c>
       <c r="L153">
@@ -10072,7 +10074,7 @@
       <c r="F154" t="s">
         <v>36</v>
       </c>
-      <c r="G154" s="12" t="s">
+      <c r="G154" t="s">
         <v>179</v>
       </c>
       <c r="H154">
@@ -10084,7 +10086,7 @@
       <c r="J154" t="s">
         <v>45</v>
       </c>
-      <c r="K154" s="12" t="s">
+      <c r="K154" t="s">
         <v>165</v>
       </c>
       <c r="L154">
@@ -10120,7 +10122,7 @@
       <c r="F155" t="s">
         <v>36</v>
       </c>
-      <c r="G155" s="12" t="s">
+      <c r="G155" t="s">
         <v>179</v>
       </c>
       <c r="H155">
@@ -10132,7 +10134,7 @@
       <c r="J155" t="s">
         <v>45</v>
       </c>
-      <c r="K155" s="12" t="s">
+      <c r="K155" t="s">
         <v>165</v>
       </c>
       <c r="L155">
@@ -10168,7 +10170,7 @@
       <c r="F156" t="s">
         <v>36</v>
       </c>
-      <c r="G156" s="12" t="s">
+      <c r="G156" t="s">
         <v>179</v>
       </c>
       <c r="H156">
@@ -10180,7 +10182,6 @@
       <c r="J156" t="s">
         <v>16</v>
       </c>
-      <c r="K156" s="12"/>
       <c r="L156">
         <v>225.82758147402399</v>
       </c>
@@ -10214,7 +10215,7 @@
       <c r="F157" t="s">
         <v>36</v>
       </c>
-      <c r="G157" s="12" t="s">
+      <c r="G157" t="s">
         <v>179</v>
       </c>
       <c r="H157">
@@ -10226,7 +10227,6 @@
       <c r="J157" t="s">
         <v>16</v>
       </c>
-      <c r="K157" s="12"/>
       <c r="L157">
         <v>236.93586718735</v>
       </c>
@@ -10260,7 +10260,7 @@
       <c r="F158" t="s">
         <v>36</v>
       </c>
-      <c r="G158" s="12" t="s">
+      <c r="G158" t="s">
         <v>179</v>
       </c>
       <c r="H158">
@@ -10272,7 +10272,6 @@
       <c r="J158" t="s">
         <v>16</v>
       </c>
-      <c r="K158" s="12"/>
       <c r="L158">
         <v>241.48529086561999</v>
       </c>
@@ -10306,7 +10305,7 @@
       <c r="F159" t="s">
         <v>36</v>
       </c>
-      <c r="G159" s="12" t="s">
+      <c r="G159" t="s">
         <v>179</v>
       </c>
       <c r="H159">
@@ -10318,7 +10317,6 @@
       <c r="J159" t="s">
         <v>16</v>
       </c>
-      <c r="K159" s="12"/>
       <c r="L159">
         <v>313.95626619498898</v>
       </c>
@@ -10352,7 +10350,7 @@
       <c r="F160" t="s">
         <v>36</v>
       </c>
-      <c r="G160" s="12" t="s">
+      <c r="G160" t="s">
         <v>179</v>
       </c>
       <c r="H160">
@@ -10364,7 +10362,6 @@
       <c r="J160" t="s">
         <v>16</v>
       </c>
-      <c r="K160" s="12"/>
       <c r="L160">
         <v>291.26267903046897</v>
       </c>
@@ -10398,7 +10395,7 @@
       <c r="F161" t="s">
         <v>36</v>
       </c>
-      <c r="G161" s="12" t="s">
+      <c r="G161" t="s">
         <v>179</v>
       </c>
       <c r="H161">
@@ -10410,7 +10407,6 @@
       <c r="J161" t="s">
         <v>16</v>
       </c>
-      <c r="K161" s="12"/>
       <c r="L161">
         <v>290.82615161212198</v>
       </c>
@@ -10444,7 +10440,7 @@
       <c r="F162" t="s">
         <v>36</v>
       </c>
-      <c r="G162" s="12" t="s">
+      <c r="G162" t="s">
         <v>179</v>
       </c>
       <c r="H162">
@@ -10456,7 +10452,6 @@
       <c r="J162" t="s">
         <v>16</v>
       </c>
-      <c r="K162" s="12"/>
       <c r="L162">
         <v>665</v>
       </c>
@@ -10493,7 +10488,7 @@
       <c r="F163" t="s">
         <v>36</v>
       </c>
-      <c r="G163" s="12" t="s">
+      <c r="G163" t="s">
         <v>179</v>
       </c>
       <c r="H163">
@@ -10505,7 +10500,7 @@
       <c r="J163" t="s">
         <v>45</v>
       </c>
-      <c r="K163" s="12" t="s">
+      <c r="K163" t="s">
         <v>165</v>
       </c>
       <c r="L163">
@@ -10544,7 +10539,7 @@
       <c r="F164" t="s">
         <v>36</v>
       </c>
-      <c r="G164" s="12" t="s">
+      <c r="G164" t="s">
         <v>179</v>
       </c>
       <c r="H164">
@@ -10556,7 +10551,6 @@
       <c r="J164" t="s">
         <v>16</v>
       </c>
-      <c r="K164" s="12"/>
       <c r="L164">
         <v>883</v>
       </c>
@@ -10593,7 +10587,7 @@
       <c r="F165" t="s">
         <v>36</v>
       </c>
-      <c r="G165" s="12" t="s">
+      <c r="G165" t="s">
         <v>179</v>
       </c>
       <c r="H165">
@@ -10605,7 +10599,7 @@
       <c r="J165" t="s">
         <v>45</v>
       </c>
-      <c r="K165" s="12" t="s">
+      <c r="K165" t="s">
         <v>165</v>
       </c>
       <c r="L165">
@@ -10644,7 +10638,7 @@
       <c r="F166" t="s">
         <v>36</v>
       </c>
-      <c r="G166" s="12" t="s">
+      <c r="G166" t="s">
         <v>179</v>
       </c>
       <c r="H166">
@@ -10656,7 +10650,6 @@
       <c r="J166" t="s">
         <v>16</v>
       </c>
-      <c r="K166" s="12"/>
       <c r="L166">
         <v>654</v>
       </c>
@@ -10693,7 +10686,7 @@
       <c r="F167" t="s">
         <v>36</v>
       </c>
-      <c r="G167" s="12" t="s">
+      <c r="G167" t="s">
         <v>179</v>
       </c>
       <c r="H167">
@@ -10705,7 +10698,7 @@
       <c r="J167" t="s">
         <v>45</v>
       </c>
-      <c r="K167" s="12" t="s">
+      <c r="K167" t="s">
         <v>165</v>
       </c>
       <c r="L167">
@@ -10744,7 +10737,7 @@
       <c r="F168" t="s">
         <v>36</v>
       </c>
-      <c r="G168" s="12" t="s">
+      <c r="G168" t="s">
         <v>179</v>
       </c>
       <c r="H168">
@@ -10756,7 +10749,6 @@
       <c r="J168" t="s">
         <v>16</v>
       </c>
-      <c r="K168" s="12"/>
       <c r="L168">
         <v>845</v>
       </c>
@@ -10793,7 +10785,7 @@
       <c r="F169" t="s">
         <v>36</v>
       </c>
-      <c r="G169" s="12" t="s">
+      <c r="G169" t="s">
         <v>179</v>
       </c>
       <c r="H169">
@@ -10805,7 +10797,7 @@
       <c r="J169" t="s">
         <v>45</v>
       </c>
-      <c r="K169" s="12" t="s">
+      <c r="K169" t="s">
         <v>165</v>
       </c>
       <c r="L169">
@@ -10844,7 +10836,7 @@
       <c r="F170" t="s">
         <v>36</v>
       </c>
-      <c r="G170" s="12" t="s">
+      <c r="G170" t="s">
         <v>179</v>
       </c>
       <c r="H170">
@@ -10856,7 +10848,6 @@
       <c r="J170" t="s">
         <v>16</v>
       </c>
-      <c r="K170" s="12"/>
       <c r="L170">
         <v>589</v>
       </c>
@@ -10893,7 +10884,7 @@
       <c r="F171" t="s">
         <v>36</v>
       </c>
-      <c r="G171" s="12" t="s">
+      <c r="G171" t="s">
         <v>179</v>
       </c>
       <c r="H171">
@@ -10905,7 +10896,7 @@
       <c r="J171" t="s">
         <v>45</v>
       </c>
-      <c r="K171" s="12" t="s">
+      <c r="K171" t="s">
         <v>165</v>
       </c>
       <c r="L171">
@@ -10944,7 +10935,7 @@
       <c r="F172" t="s">
         <v>36</v>
       </c>
-      <c r="G172" s="12" t="s">
+      <c r="G172" t="s">
         <v>179</v>
       </c>
       <c r="H172">
@@ -10956,7 +10947,6 @@
       <c r="J172" t="s">
         <v>16</v>
       </c>
-      <c r="K172" s="12"/>
       <c r="L172">
         <v>592</v>
       </c>
@@ -10993,7 +10983,7 @@
       <c r="F173" t="s">
         <v>36</v>
       </c>
-      <c r="G173" s="12" t="s">
+      <c r="G173" t="s">
         <v>179</v>
       </c>
       <c r="H173">
@@ -11005,7 +10995,7 @@
       <c r="J173" t="s">
         <v>45</v>
       </c>
-      <c r="K173" s="12" t="s">
+      <c r="K173" t="s">
         <v>165</v>
       </c>
       <c r="L173">
@@ -11044,7 +11034,7 @@
       <c r="F174" t="s">
         <v>36</v>
       </c>
-      <c r="G174" s="12" t="s">
+      <c r="G174" t="s">
         <v>179</v>
       </c>
       <c r="H174">
@@ -11056,7 +11046,6 @@
       <c r="J174" t="s">
         <v>16</v>
       </c>
-      <c r="K174" s="12"/>
       <c r="L174">
         <v>732</v>
       </c>
@@ -11093,7 +11082,7 @@
       <c r="F175" t="s">
         <v>36</v>
       </c>
-      <c r="G175" s="12" t="s">
+      <c r="G175" t="s">
         <v>179</v>
       </c>
       <c r="H175">
@@ -11105,7 +11094,7 @@
       <c r="J175" t="s">
         <v>45</v>
       </c>
-      <c r="K175" s="12" t="s">
+      <c r="K175" t="s">
         <v>165</v>
       </c>
       <c r="L175">
@@ -11144,7 +11133,7 @@
       <c r="F176" t="s">
         <v>36</v>
       </c>
-      <c r="G176" s="12" t="s">
+      <c r="G176" t="s">
         <v>179</v>
       </c>
       <c r="H176">
@@ -11156,7 +11145,6 @@
       <c r="J176" t="s">
         <v>16</v>
       </c>
-      <c r="K176" s="12"/>
       <c r="L176">
         <v>607</v>
       </c>
@@ -11193,7 +11181,7 @@
       <c r="F177" t="s">
         <v>36</v>
       </c>
-      <c r="G177" s="12" t="s">
+      <c r="G177" t="s">
         <v>179</v>
       </c>
       <c r="H177">
@@ -11205,7 +11193,7 @@
       <c r="J177" t="s">
         <v>45</v>
       </c>
-      <c r="K177" s="12" t="s">
+      <c r="K177" t="s">
         <v>165</v>
       </c>
       <c r="L177">
@@ -11259,11 +11247,11 @@
       <c r="K178" t="s">
         <v>198</v>
       </c>
-      <c r="L178" s="14">
+      <c r="L178" s="13">
         <v>256.39999999999998</v>
       </c>
-      <c r="M178" s="15"/>
-      <c r="N178" s="14">
+      <c r="M178" s="14"/>
+      <c r="N178" s="13">
         <v>214.2</v>
       </c>
       <c r="O178">
@@ -11272,7 +11260,7 @@
       <c r="P178" t="s">
         <v>10</v>
       </c>
-      <c r="Q178" s="13">
+      <c r="Q178" s="12">
         <v>78</v>
       </c>
     </row>
@@ -11311,11 +11299,11 @@
       <c r="K179" t="s">
         <v>198</v>
       </c>
-      <c r="L179" s="14">
+      <c r="L179" s="13">
         <v>424.3</v>
       </c>
-      <c r="M179" s="15"/>
-      <c r="N179" s="14">
+      <c r="M179" s="14"/>
+      <c r="N179" s="13">
         <v>332</v>
       </c>
       <c r="O179">
@@ -11324,7 +11312,7 @@
       <c r="P179" t="s">
         <v>11</v>
       </c>
-      <c r="Q179" s="13">
+      <c r="Q179" s="12">
         <v>78</v>
       </c>
     </row>
@@ -11363,11 +11351,11 @@
       <c r="K180" t="s">
         <v>198</v>
       </c>
-      <c r="L180" s="14">
+      <c r="L180" s="13">
         <v>316.7</v>
       </c>
-      <c r="M180" s="15"/>
-      <c r="N180" s="14">
+      <c r="M180" s="14"/>
+      <c r="N180" s="13">
         <v>266.3</v>
       </c>
       <c r="O180">
@@ -11376,7 +11364,7 @@
       <c r="P180" t="s">
         <v>10</v>
       </c>
-      <c r="Q180" s="13">
+      <c r="Q180" s="12">
         <v>78</v>
       </c>
     </row>
@@ -11415,11 +11403,11 @@
       <c r="K181" t="s">
         <v>198</v>
       </c>
-      <c r="L181" s="14">
+      <c r="L181" s="13">
         <v>517.70000000000005</v>
       </c>
-      <c r="M181" s="15"/>
-      <c r="N181" s="14">
+      <c r="M181" s="14"/>
+      <c r="N181" s="13">
         <v>407.4</v>
       </c>
       <c r="O181">
@@ -11428,7 +11416,7 @@
       <c r="P181" t="s">
         <v>11</v>
       </c>
-      <c r="Q181" s="13">
+      <c r="Q181" s="12">
         <v>78</v>
       </c>
     </row>
@@ -11467,11 +11455,11 @@
       <c r="K182" t="s">
         <v>198</v>
       </c>
-      <c r="L182" s="14">
+      <c r="L182" s="13">
         <v>300.5</v>
       </c>
-      <c r="M182" s="15"/>
-      <c r="N182" s="14">
+      <c r="M182" s="14"/>
+      <c r="N182" s="13">
         <v>251.7</v>
       </c>
       <c r="O182">
@@ -11480,7 +11468,7 @@
       <c r="P182" t="s">
         <v>10</v>
       </c>
-      <c r="Q182" s="13">
+      <c r="Q182" s="12">
         <v>78</v>
       </c>
     </row>
@@ -11519,11 +11507,11 @@
       <c r="K183" t="s">
         <v>198</v>
       </c>
-      <c r="L183" s="14">
+      <c r="L183" s="13">
         <v>506.1</v>
       </c>
-      <c r="M183" s="15"/>
-      <c r="N183" s="14">
+      <c r="M183" s="14"/>
+      <c r="N183" s="13">
         <v>395</v>
       </c>
       <c r="O183">
@@ -11532,7 +11520,7 @@
       <c r="P183" t="s">
         <v>11</v>
       </c>
-      <c r="Q183" s="13">
+      <c r="Q183" s="12">
         <v>78</v>
       </c>
     </row>
@@ -11571,11 +11559,11 @@
       <c r="K184" t="s">
         <v>198</v>
       </c>
-      <c r="L184" s="14">
+      <c r="L184" s="13">
         <v>244</v>
       </c>
-      <c r="M184" s="15"/>
-      <c r="N184" s="14">
+      <c r="M184" s="14"/>
+      <c r="N184" s="13">
         <v>202.6</v>
       </c>
       <c r="O184">
@@ -11584,7 +11572,7 @@
       <c r="P184" t="s">
         <v>10</v>
       </c>
-      <c r="Q184" s="13">
+      <c r="Q184" s="12">
         <v>78</v>
       </c>
     </row>
@@ -11623,11 +11611,11 @@
       <c r="K185" t="s">
         <v>198</v>
       </c>
-      <c r="L185" s="14">
+      <c r="L185" s="13">
         <v>570.6</v>
       </c>
-      <c r="M185" s="15"/>
-      <c r="N185" s="14">
+      <c r="M185" s="14"/>
+      <c r="N185" s="13">
         <v>453.7</v>
       </c>
       <c r="O185">
@@ -11636,7 +11624,7 @@
       <c r="P185" t="s">
         <v>11</v>
       </c>
-      <c r="Q185" s="13">
+      <c r="Q185" s="12">
         <v>78</v>
       </c>
     </row>
@@ -11675,11 +11663,11 @@
       <c r="K186" t="s">
         <v>198</v>
       </c>
-      <c r="L186" s="14">
+      <c r="L186" s="13">
         <v>208</v>
       </c>
-      <c r="M186" s="15"/>
-      <c r="N186" s="14">
+      <c r="M186" s="14"/>
+      <c r="N186" s="13">
         <v>180</v>
       </c>
       <c r="O186">
@@ -11688,7 +11676,7 @@
       <c r="P186" t="s">
         <v>10</v>
       </c>
-      <c r="Q186" s="13">
+      <c r="Q186" s="12">
         <v>89</v>
       </c>
     </row>
@@ -11727,11 +11715,11 @@
       <c r="K187" t="s">
         <v>198</v>
       </c>
-      <c r="L187" s="14">
+      <c r="L187" s="13">
         <v>364.9</v>
       </c>
-      <c r="M187" s="15"/>
-      <c r="N187" s="14">
+      <c r="M187" s="14"/>
+      <c r="N187" s="13">
         <v>285.60000000000002</v>
       </c>
       <c r="O187">
@@ -11740,7 +11728,7 @@
       <c r="P187" t="s">
         <v>11</v>
       </c>
-      <c r="Q187" s="13">
+      <c r="Q187" s="12">
         <v>89</v>
       </c>
     </row>
@@ -11779,11 +11767,11 @@
       <c r="K188" t="s">
         <v>198</v>
       </c>
-      <c r="L188" s="14">
+      <c r="L188" s="13">
         <v>259.8</v>
       </c>
-      <c r="M188" s="15"/>
-      <c r="N188" s="14">
+      <c r="M188" s="14"/>
+      <c r="N188" s="13">
         <v>222.5</v>
       </c>
       <c r="O188">
@@ -11792,7 +11780,7 @@
       <c r="P188" t="s">
         <v>10</v>
       </c>
-      <c r="Q188" s="13">
+      <c r="Q188" s="12">
         <v>89</v>
       </c>
     </row>
@@ -11831,11 +11819,11 @@
       <c r="K189" t="s">
         <v>198</v>
       </c>
-      <c r="L189" s="14">
+      <c r="L189" s="13">
         <v>464.5</v>
       </c>
-      <c r="M189" s="15"/>
-      <c r="N189" s="14">
+      <c r="M189" s="14"/>
+      <c r="N189" s="13">
         <v>363.7</v>
       </c>
       <c r="O189">
@@ -11844,7 +11832,7 @@
       <c r="P189" t="s">
         <v>11</v>
       </c>
-      <c r="Q189" s="13">
+      <c r="Q189" s="12">
         <v>89</v>
       </c>
     </row>
@@ -11883,11 +11871,11 @@
       <c r="K190" t="s">
         <v>198</v>
       </c>
-      <c r="L190" s="14">
+      <c r="L190" s="13">
         <v>278.89999999999998</v>
       </c>
-      <c r="M190" s="15"/>
-      <c r="N190" s="14">
+      <c r="M190" s="14"/>
+      <c r="N190" s="13">
         <v>239.2</v>
       </c>
       <c r="O190">
@@ -11896,7 +11884,7 @@
       <c r="P190" t="s">
         <v>10</v>
       </c>
-      <c r="Q190" s="13">
+      <c r="Q190" s="12">
         <v>89</v>
       </c>
     </row>
@@ -11935,11 +11923,11 @@
       <c r="K191" t="s">
         <v>198</v>
       </c>
-      <c r="L191" s="14">
+      <c r="L191" s="13">
         <v>507.4</v>
       </c>
-      <c r="M191" s="15"/>
-      <c r="N191" s="14">
+      <c r="M191" s="14"/>
+      <c r="N191" s="13">
         <v>396.4</v>
       </c>
       <c r="O191">
@@ -11948,7 +11936,7 @@
       <c r="P191" t="s">
         <v>11</v>
       </c>
-      <c r="Q191" s="13">
+      <c r="Q191" s="12">
         <v>89</v>
       </c>
     </row>
@@ -11987,11 +11975,11 @@
       <c r="K192" t="s">
         <v>198</v>
       </c>
-      <c r="L192" s="14">
+      <c r="L192" s="13">
         <v>205.4</v>
       </c>
-      <c r="M192" s="15"/>
-      <c r="N192" s="14">
+      <c r="M192" s="14"/>
+      <c r="N192" s="13">
         <v>175.5</v>
       </c>
       <c r="O192">
@@ -12000,7 +11988,7 @@
       <c r="P192" t="s">
         <v>10</v>
       </c>
-      <c r="Q192" s="13">
+      <c r="Q192" s="12">
         <v>89</v>
       </c>
     </row>
@@ -12039,11 +12027,11 @@
       <c r="K193" t="s">
         <v>198</v>
       </c>
-      <c r="L193" s="14">
+      <c r="L193" s="13">
         <v>458.1</v>
       </c>
-      <c r="M193" s="15"/>
-      <c r="N193" s="14">
+      <c r="M193" s="14"/>
+      <c r="N193" s="13">
         <v>361.9</v>
       </c>
       <c r="O193">
@@ -12052,7 +12040,7 @@
       <c r="P193" t="s">
         <v>11</v>
       </c>
-      <c r="Q193" s="13">
+      <c r="Q193" s="12">
         <v>89</v>
       </c>
     </row>
@@ -12091,11 +12079,11 @@
       <c r="K194" t="s">
         <v>199</v>
       </c>
-      <c r="L194" s="14">
+      <c r="L194" s="13">
         <v>234.9</v>
       </c>
-      <c r="M194" s="15"/>
-      <c r="N194" s="14">
+      <c r="M194" s="14"/>
+      <c r="N194" s="13">
         <v>200.4</v>
       </c>
       <c r="O194">
@@ -12104,7 +12092,7 @@
       <c r="P194" t="s">
         <v>10</v>
       </c>
-      <c r="Q194" s="13">
+      <c r="Q194" s="12">
         <v>80</v>
       </c>
     </row>
@@ -12143,11 +12131,11 @@
       <c r="K195" t="s">
         <v>199</v>
       </c>
-      <c r="L195" s="14">
+      <c r="L195" s="13">
         <v>426.9</v>
       </c>
-      <c r="M195" s="15"/>
-      <c r="N195" s="14">
+      <c r="M195" s="14"/>
+      <c r="N195" s="13">
         <v>331.7</v>
       </c>
       <c r="O195">
@@ -12156,7 +12144,7 @@
       <c r="P195" t="s">
         <v>11</v>
       </c>
-      <c r="Q195" s="13">
+      <c r="Q195" s="12">
         <v>80</v>
       </c>
     </row>
@@ -12195,11 +12183,11 @@
       <c r="K196" t="s">
         <v>199</v>
       </c>
-      <c r="L196" s="14">
+      <c r="L196" s="13">
         <v>356.9</v>
       </c>
-      <c r="M196" s="15"/>
-      <c r="N196" s="14">
+      <c r="M196" s="14"/>
+      <c r="N196" s="13">
         <v>298.8</v>
       </c>
       <c r="O196">
@@ -12208,7 +12196,7 @@
       <c r="P196" t="s">
         <v>10</v>
       </c>
-      <c r="Q196" s="13">
+      <c r="Q196" s="12">
         <v>80</v>
       </c>
     </row>
@@ -12247,11 +12235,11 @@
       <c r="K197" t="s">
         <v>199</v>
       </c>
-      <c r="L197" s="14">
+      <c r="L197" s="13">
         <v>688.6</v>
       </c>
-      <c r="M197" s="15"/>
-      <c r="N197" s="14">
+      <c r="M197" s="14"/>
+      <c r="N197" s="13">
         <v>528.6</v>
       </c>
       <c r="O197">
@@ -12260,7 +12248,7 @@
       <c r="P197" t="s">
         <v>11</v>
       </c>
-      <c r="Q197" s="13">
+      <c r="Q197" s="12">
         <v>80</v>
       </c>
     </row>
@@ -12299,11 +12287,11 @@
       <c r="K198" t="s">
         <v>199</v>
       </c>
-      <c r="L198" s="14">
+      <c r="L198" s="13">
         <v>311.89999999999998</v>
       </c>
-      <c r="M198" s="15"/>
-      <c r="N198" s="14">
+      <c r="M198" s="14"/>
+      <c r="N198" s="13">
         <v>261.7</v>
       </c>
       <c r="O198">
@@ -12312,7 +12300,7 @@
       <c r="P198" t="s">
         <v>10</v>
       </c>
-      <c r="Q198" s="13">
+      <c r="Q198" s="12">
         <v>80</v>
       </c>
     </row>
@@ -12351,11 +12339,11 @@
       <c r="K199" t="s">
         <v>199</v>
       </c>
-      <c r="L199" s="14">
+      <c r="L199" s="13">
         <v>615.1</v>
       </c>
-      <c r="M199" s="15"/>
-      <c r="N199" s="14">
+      <c r="M199" s="14"/>
+      <c r="N199" s="13">
         <v>468.9</v>
       </c>
       <c r="O199">
@@ -12364,7 +12352,7 @@
       <c r="P199" t="s">
         <v>11</v>
       </c>
-      <c r="Q199" s="13">
+      <c r="Q199" s="12">
         <v>80</v>
       </c>
     </row>
@@ -12403,11 +12391,11 @@
       <c r="K200" t="s">
         <v>199</v>
       </c>
-      <c r="L200" s="14">
+      <c r="L200" s="13">
         <v>228.2</v>
       </c>
-      <c r="M200" s="15"/>
-      <c r="N200" s="14">
+      <c r="M200" s="14"/>
+      <c r="N200" s="13">
         <v>193.8</v>
       </c>
       <c r="O200">
@@ -12416,7 +12404,7 @@
       <c r="P200" t="s">
         <v>10</v>
       </c>
-      <c r="Q200" s="13">
+      <c r="Q200" s="12">
         <v>80</v>
       </c>
     </row>
@@ -12455,11 +12443,11 @@
       <c r="K201" t="s">
         <v>199</v>
       </c>
-      <c r="L201" s="14">
+      <c r="L201" s="13">
         <v>606.1</v>
       </c>
-      <c r="M201" s="15"/>
-      <c r="N201" s="14">
+      <c r="M201" s="14"/>
+      <c r="N201" s="13">
         <v>479.9</v>
       </c>
       <c r="O201">
@@ -12468,7 +12456,7 @@
       <c r="P201" t="s">
         <v>11</v>
       </c>
-      <c r="Q201" s="13">
+      <c r="Q201" s="12">
         <v>80</v>
       </c>
     </row>
@@ -12507,11 +12495,11 @@
       <c r="K202" t="s">
         <v>199</v>
       </c>
-      <c r="L202" s="15">
+      <c r="L202" s="14">
         <v>276.39999999999998</v>
       </c>
-      <c r="M202" s="15"/>
-      <c r="N202" s="15">
+      <c r="M202" s="14"/>
+      <c r="N202" s="14">
         <v>235.9</v>
       </c>
       <c r="O202">
@@ -12559,11 +12547,11 @@
       <c r="K203" t="s">
         <v>199</v>
       </c>
-      <c r="L203" s="15">
+      <c r="L203" s="14">
         <v>498.6</v>
       </c>
-      <c r="M203" s="15"/>
-      <c r="N203" s="15">
+      <c r="M203" s="14"/>
+      <c r="N203" s="14">
         <v>395.6</v>
       </c>
       <c r="O203">
@@ -12611,11 +12599,11 @@
       <c r="K204" t="s">
         <v>199</v>
       </c>
-      <c r="L204" s="15">
+      <c r="L204" s="14">
         <v>398.8</v>
       </c>
-      <c r="M204" s="15"/>
-      <c r="N204" s="15">
+      <c r="M204" s="14"/>
+      <c r="N204" s="14">
         <v>340.8</v>
       </c>
       <c r="O204">
@@ -12663,11 +12651,11 @@
       <c r="K205" t="s">
         <v>199</v>
       </c>
-      <c r="L205" s="15">
+      <c r="L205" s="14">
         <v>638.20000000000005</v>
       </c>
-      <c r="M205" s="15"/>
-      <c r="N205" s="15">
+      <c r="M205" s="14"/>
+      <c r="N205" s="14">
         <v>510.9</v>
       </c>
       <c r="O205">
@@ -12715,11 +12703,11 @@
       <c r="K206" t="s">
         <v>199</v>
       </c>
-      <c r="L206" s="15">
+      <c r="L206" s="14">
         <v>373.3</v>
       </c>
-      <c r="M206" s="15"/>
-      <c r="N206" s="15">
+      <c r="M206" s="14"/>
+      <c r="N206" s="14">
         <v>320.89999999999998</v>
       </c>
       <c r="O206">
@@ -12767,11 +12755,11 @@
       <c r="K207" t="s">
         <v>199</v>
       </c>
-      <c r="L207" s="15">
+      <c r="L207" s="14">
         <v>674.3</v>
       </c>
-      <c r="M207" s="15"/>
-      <c r="N207" s="15">
+      <c r="M207" s="14"/>
+      <c r="N207" s="14">
         <v>544.9</v>
       </c>
       <c r="O207">
@@ -12819,11 +12807,11 @@
       <c r="K208" t="s">
         <v>199</v>
       </c>
-      <c r="L208" s="15">
+      <c r="L208" s="14">
         <v>266.7</v>
       </c>
-      <c r="M208" s="15"/>
-      <c r="N208" s="15">
+      <c r="M208" s="14"/>
+      <c r="N208" s="14">
         <v>228.6</v>
       </c>
       <c r="O208">
@@ -12871,11 +12859,11 @@
       <c r="K209" t="s">
         <v>199</v>
       </c>
-      <c r="L209" s="15">
+      <c r="L209" s="14">
         <v>583.20000000000005</v>
       </c>
-      <c r="M209" s="15"/>
-      <c r="N209" s="15">
+      <c r="M209" s="14"/>
+      <c r="N209" s="14">
         <v>471.2</v>
       </c>
       <c r="O209">
@@ -12920,11 +12908,11 @@
       <c r="J210" t="s">
         <v>16</v>
       </c>
-      <c r="L210" s="15">
+      <c r="L210" s="14">
         <v>251.7</v>
       </c>
-      <c r="M210" s="15"/>
-      <c r="N210" s="15">
+      <c r="M210" s="14"/>
+      <c r="N210" s="14">
         <v>213.7</v>
       </c>
       <c r="O210">
@@ -12969,11 +12957,11 @@
       <c r="J211" t="s">
         <v>16</v>
       </c>
-      <c r="L211" s="15">
+      <c r="L211" s="14">
         <v>477.5</v>
       </c>
-      <c r="M211" s="15"/>
-      <c r="N211" s="15">
+      <c r="M211" s="14"/>
+      <c r="N211" s="14">
         <v>361.3</v>
       </c>
       <c r="O211">
@@ -13018,11 +13006,11 @@
       <c r="J212" t="s">
         <v>16</v>
       </c>
-      <c r="L212" s="15">
+      <c r="L212" s="14">
         <v>235</v>
       </c>
-      <c r="M212" s="15"/>
-      <c r="N212" s="15">
+      <c r="M212" s="14"/>
+      <c r="N212" s="14">
         <v>202.1</v>
       </c>
       <c r="O212">
@@ -13067,11 +13055,11 @@
       <c r="J213" t="s">
         <v>16</v>
       </c>
-      <c r="L213" s="15">
+      <c r="L213" s="14">
         <v>441.4</v>
       </c>
-      <c r="M213" s="15"/>
-      <c r="N213" s="15">
+      <c r="M213" s="14"/>
+      <c r="N213" s="14">
         <v>331.6</v>
       </c>
       <c r="O213">
@@ -13116,11 +13104,11 @@
       <c r="J214" t="s">
         <v>16</v>
       </c>
-      <c r="L214" s="15">
+      <c r="L214" s="14">
         <v>229.3</v>
       </c>
-      <c r="M214" s="15"/>
-      <c r="N214" s="15">
+      <c r="M214" s="14"/>
+      <c r="N214" s="14">
         <v>195.2</v>
       </c>
       <c r="O214">
@@ -13165,11 +13153,11 @@
       <c r="J215" t="s">
         <v>16</v>
       </c>
-      <c r="L215" s="15">
+      <c r="L215" s="14">
         <v>454</v>
       </c>
-      <c r="M215" s="15"/>
-      <c r="N215" s="15">
+      <c r="M215" s="14"/>
+      <c r="N215" s="14">
         <v>340.7</v>
       </c>
       <c r="O215">
@@ -13214,11 +13202,11 @@
       <c r="J216" t="s">
         <v>16</v>
       </c>
-      <c r="L216" s="15">
+      <c r="L216" s="14">
         <v>202.2</v>
       </c>
-      <c r="M216" s="15"/>
-      <c r="N216" s="15">
+      <c r="M216" s="14"/>
+      <c r="N216" s="14">
         <v>172.4</v>
       </c>
       <c r="O216">
@@ -13263,11 +13251,11 @@
       <c r="J217" t="s">
         <v>16</v>
       </c>
-      <c r="L217" s="15">
+      <c r="L217" s="14">
         <v>518.1</v>
       </c>
-      <c r="M217" s="15"/>
-      <c r="N217" s="15">
+      <c r="M217" s="14"/>
+      <c r="N217" s="14">
         <v>398.7</v>
       </c>
       <c r="O217">
@@ -13312,11 +13300,11 @@
       <c r="J218" t="s">
         <v>16</v>
       </c>
-      <c r="L218" s="15">
+      <c r="L218" s="14">
         <v>251.7</v>
       </c>
-      <c r="M218" s="15"/>
-      <c r="N218" s="15">
+      <c r="M218" s="14"/>
+      <c r="N218" s="14">
         <v>213.7</v>
       </c>
       <c r="O218">
@@ -13361,11 +13349,11 @@
       <c r="J219" t="s">
         <v>16</v>
       </c>
-      <c r="L219" s="15">
+      <c r="L219" s="14">
         <v>477.5</v>
       </c>
-      <c r="M219" s="15"/>
-      <c r="N219" s="15">
+      <c r="M219" s="14"/>
+      <c r="N219" s="14">
         <v>361.3</v>
       </c>
       <c r="O219">
@@ -13410,11 +13398,11 @@
       <c r="J220" t="s">
         <v>16</v>
       </c>
-      <c r="L220" s="15">
+      <c r="L220" s="14">
         <v>235</v>
       </c>
-      <c r="M220" s="15"/>
-      <c r="N220" s="15">
+      <c r="M220" s="14"/>
+      <c r="N220" s="14">
         <v>202.1</v>
       </c>
       <c r="O220">
@@ -13459,11 +13447,11 @@
       <c r="J221" t="s">
         <v>16</v>
       </c>
-      <c r="L221" s="15">
+      <c r="L221" s="14">
         <v>441.4</v>
       </c>
-      <c r="M221" s="15"/>
-      <c r="N221" s="15">
+      <c r="M221" s="14"/>
+      <c r="N221" s="14">
         <v>331.6</v>
       </c>
       <c r="O221">
@@ -13508,11 +13496,11 @@
       <c r="J222" t="s">
         <v>16</v>
       </c>
-      <c r="L222" s="15">
+      <c r="L222" s="14">
         <v>229.3</v>
       </c>
-      <c r="M222" s="15"/>
-      <c r="N222" s="15">
+      <c r="M222" s="14"/>
+      <c r="N222" s="14">
         <v>195.2</v>
       </c>
       <c r="O222">
@@ -13557,11 +13545,11 @@
       <c r="J223" t="s">
         <v>16</v>
       </c>
-      <c r="L223" s="15">
+      <c r="L223" s="14">
         <v>454</v>
       </c>
-      <c r="M223" s="15"/>
-      <c r="N223" s="15">
+      <c r="M223" s="14"/>
+      <c r="N223" s="14">
         <v>340.7</v>
       </c>
       <c r="O223">
@@ -13606,11 +13594,11 @@
       <c r="J224" t="s">
         <v>16</v>
       </c>
-      <c r="L224" s="15">
+      <c r="L224" s="14">
         <v>202.2</v>
       </c>
-      <c r="M224" s="15"/>
-      <c r="N224" s="15">
+      <c r="M224" s="14"/>
+      <c r="N224" s="14">
         <v>172.4</v>
       </c>
       <c r="O224">
@@ -13655,11 +13643,11 @@
       <c r="J225" t="s">
         <v>16</v>
       </c>
-      <c r="L225" s="15">
+      <c r="L225" s="14">
         <v>518.1</v>
       </c>
-      <c r="M225" s="15"/>
-      <c r="N225" s="15">
+      <c r="M225" s="14"/>
+      <c r="N225" s="14">
         <v>398.7</v>
       </c>
       <c r="O225">
@@ -13704,11 +13692,11 @@
       <c r="J226" t="s">
         <v>16</v>
       </c>
-      <c r="L226" s="15">
+      <c r="L226" s="14">
         <v>251.7</v>
       </c>
-      <c r="M226" s="15"/>
-      <c r="N226" s="15">
+      <c r="M226" s="14"/>
+      <c r="N226" s="14">
         <v>213.7</v>
       </c>
       <c r="O226">
@@ -13753,11 +13741,11 @@
       <c r="J227" t="s">
         <v>16</v>
       </c>
-      <c r="L227" s="15">
+      <c r="L227" s="14">
         <v>477.5</v>
       </c>
-      <c r="M227" s="15"/>
-      <c r="N227" s="15">
+      <c r="M227" s="14"/>
+      <c r="N227" s="14">
         <v>361.3</v>
       </c>
       <c r="O227">
@@ -13802,11 +13790,11 @@
       <c r="J228" t="s">
         <v>16</v>
       </c>
-      <c r="L228" s="15">
+      <c r="L228" s="14">
         <v>235</v>
       </c>
-      <c r="M228" s="15"/>
-      <c r="N228" s="15">
+      <c r="M228" s="14"/>
+      <c r="N228" s="14">
         <v>202.1</v>
       </c>
       <c r="O228">
@@ -13851,11 +13839,11 @@
       <c r="J229" t="s">
         <v>16</v>
       </c>
-      <c r="L229" s="15">
+      <c r="L229" s="14">
         <v>441.4</v>
       </c>
-      <c r="M229" s="15"/>
-      <c r="N229" s="15">
+      <c r="M229" s="14"/>
+      <c r="N229" s="14">
         <v>331.6</v>
       </c>
       <c r="O229">
@@ -13900,11 +13888,11 @@
       <c r="J230" t="s">
         <v>16</v>
       </c>
-      <c r="L230" s="15">
+      <c r="L230" s="14">
         <v>229.3</v>
       </c>
-      <c r="M230" s="15"/>
-      <c r="N230" s="15">
+      <c r="M230" s="14"/>
+      <c r="N230" s="14">
         <v>195.2</v>
       </c>
       <c r="O230">
@@ -13949,11 +13937,11 @@
       <c r="J231" t="s">
         <v>16</v>
       </c>
-      <c r="L231" s="15">
+      <c r="L231" s="14">
         <v>454</v>
       </c>
-      <c r="M231" s="15"/>
-      <c r="N231" s="15">
+      <c r="M231" s="14"/>
+      <c r="N231" s="14">
         <v>340.7</v>
       </c>
       <c r="O231">
@@ -13998,11 +13986,11 @@
       <c r="J232" t="s">
         <v>16</v>
       </c>
-      <c r="L232" s="15">
+      <c r="L232" s="14">
         <v>202.2</v>
       </c>
-      <c r="M232" s="15"/>
-      <c r="N232" s="15">
+      <c r="M232" s="14"/>
+      <c r="N232" s="14">
         <v>172.4</v>
       </c>
       <c r="O232">
@@ -14047,11 +14035,11 @@
       <c r="J233" t="s">
         <v>16</v>
       </c>
-      <c r="L233" s="15">
+      <c r="L233" s="14">
         <v>518.1</v>
       </c>
-      <c r="M233" s="15"/>
-      <c r="N233" s="15">
+      <c r="M233" s="14"/>
+      <c r="N233" s="14">
         <v>398.7</v>
       </c>
       <c r="O233">
@@ -14096,11 +14084,11 @@
       <c r="J234" t="s">
         <v>16</v>
       </c>
-      <c r="L234" s="15">
+      <c r="L234" s="14">
         <v>251.7</v>
       </c>
-      <c r="M234" s="15"/>
-      <c r="N234" s="15">
+      <c r="M234" s="14"/>
+      <c r="N234" s="14">
         <v>213.7</v>
       </c>
       <c r="O234">
@@ -14145,11 +14133,11 @@
       <c r="J235" t="s">
         <v>16</v>
       </c>
-      <c r="L235" s="15">
+      <c r="L235" s="14">
         <v>477.5</v>
       </c>
-      <c r="M235" s="15"/>
-      <c r="N235" s="15">
+      <c r="M235" s="14"/>
+      <c r="N235" s="14">
         <v>361.3</v>
       </c>
       <c r="O235">
@@ -14194,11 +14182,11 @@
       <c r="J236" t="s">
         <v>16</v>
       </c>
-      <c r="L236" s="15">
+      <c r="L236" s="14">
         <v>235</v>
       </c>
-      <c r="M236" s="15"/>
-      <c r="N236" s="15">
+      <c r="M236" s="14"/>
+      <c r="N236" s="14">
         <v>202.1</v>
       </c>
       <c r="O236">
@@ -14243,11 +14231,11 @@
       <c r="J237" t="s">
         <v>16</v>
       </c>
-      <c r="L237" s="15">
+      <c r="L237" s="14">
         <v>441.4</v>
       </c>
-      <c r="M237" s="15"/>
-      <c r="N237" s="15">
+      <c r="M237" s="14"/>
+      <c r="N237" s="14">
         <v>331.6</v>
       </c>
       <c r="O237">
@@ -14292,11 +14280,11 @@
       <c r="J238" t="s">
         <v>16</v>
       </c>
-      <c r="L238" s="15">
+      <c r="L238" s="14">
         <v>229.3</v>
       </c>
-      <c r="M238" s="15"/>
-      <c r="N238" s="15">
+      <c r="M238" s="14"/>
+      <c r="N238" s="14">
         <v>195.2</v>
       </c>
       <c r="O238">
@@ -14341,11 +14329,11 @@
       <c r="J239" t="s">
         <v>16</v>
       </c>
-      <c r="L239" s="15">
+      <c r="L239" s="14">
         <v>454</v>
       </c>
-      <c r="M239" s="15"/>
-      <c r="N239" s="15">
+      <c r="M239" s="14"/>
+      <c r="N239" s="14">
         <v>340.7</v>
       </c>
       <c r="O239">
@@ -14390,11 +14378,11 @@
       <c r="J240" t="s">
         <v>16</v>
       </c>
-      <c r="L240" s="15">
+      <c r="L240" s="14">
         <v>202.2</v>
       </c>
-      <c r="M240" s="15"/>
-      <c r="N240" s="15">
+      <c r="M240" s="14"/>
+      <c r="N240" s="14">
         <v>172.4</v>
       </c>
       <c r="O240">
@@ -14439,11 +14427,11 @@
       <c r="J241" t="s">
         <v>16</v>
       </c>
-      <c r="L241" s="15">
+      <c r="L241" s="14">
         <v>518.1</v>
       </c>
-      <c r="M241" s="15"/>
-      <c r="N241" s="15">
+      <c r="M241" s="14"/>
+      <c r="N241" s="14">
         <v>398.7</v>
       </c>
       <c r="O241">
@@ -16216,7 +16204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62B96E09-4BF7-5E4A-9A2D-7FF2A0B754F5}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -16539,7 +16527,7 @@
       <c r="A15" t="s">
         <v>186</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" t="s">
         <v>60</v>
       </c>
       <c r="J15" t="s">
@@ -16651,8 +16639,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DC9BE8B-F6ED-034E-98E8-60BCAE861F6C}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -16679,7 +16667,7 @@
       <c r="A3" s="6" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>138</v>
       </c>
     </row>
@@ -16687,7 +16675,7 @@
       <c r="A4" s="6" t="s">
         <v>141</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="7" t="s">
         <v>140</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -16725,7 +16713,7 @@
       <c r="A8" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>155</v>
       </c>
     </row>
@@ -16745,15 +16733,18 @@
       <c r="A17" s="6" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>151</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="6" t="s">
+    <row r="18" spans="1:3" s="6" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>205</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>156</v>
       </c>
     </row>
@@ -16767,7 +16758,7 @@
       <c r="A22" t="s">
         <v>160</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="9" t="s">
         <v>158</v>
       </c>
       <c r="C22" t="s">
@@ -16779,6 +16770,12 @@
     <hyperlink ref="B5" r:id="rId1" xr:uid="{C5424597-DB1E-4C40-B96F-CBB23659F93A}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{1B2DA229-A5ED-D346-A617-A85BD17C27A5}"/>
     <hyperlink ref="B7" r:id="rId3" xr:uid="{9D68D773-2BDC-6B46-8681-23EB87CDCADF}"/>
+    <hyperlink ref="B3" r:id="rId4" xr:uid="{33DAC83A-0537-0742-B851-7D7BFFDED483}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{7A0908FB-7DAD-3A47-BAFC-047692951EAB}"/>
+    <hyperlink ref="B8" r:id="rId6" xr:uid="{C56885C6-8AAF-6548-86D9-00B9C82ACE47}"/>
+    <hyperlink ref="B17" r:id="rId7" xr:uid="{18D24FD5-E485-2642-97C4-AEAFD6C8337F}"/>
+    <hyperlink ref="B18" r:id="rId8" xr:uid="{6B33DAAA-76C7-3D4F-90EF-FA86CE5AE552}"/>
+    <hyperlink ref="B22" r:id="rId9" xr:uid="{FBDC49BD-397F-C747-8EFD-0A205CF9D6D8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>